<commit_message>
Anado la carpeta sesiones que va a contener las sesiones de entrenamiento y creo los entrenamientos de las primeras 7 sesiones
</commit_message>
<xml_diff>
--- a/planificacion/sesiones/lbh-sesiones-agosto.xlsx
+++ b/planificacion/sesiones/lbh-sesiones-agosto.xlsx
@@ -7,21 +7,21 @@
     <workbookView xWindow="120" yWindow="135" windowWidth="9420" windowHeight="4500" tabRatio="862"/>
   </bookViews>
   <sheets>
-    <sheet name="23-8" sheetId="4" r:id="rId1"/>
-    <sheet name="Hoja2" sheetId="13" r:id="rId2"/>
+    <sheet name="18-8" sheetId="13" r:id="rId1"/>
+    <sheet name="23-8" sheetId="4" r:id="rId2"/>
     <sheet name="Hoja3" sheetId="14" r:id="rId3"/>
     <sheet name="Hoja4" sheetId="15" r:id="rId4"/>
     <sheet name="PLANTILLA" sheetId="12" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'23-8'!$A$1:$K$54</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">'23-8'!$A$1:$K$54</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="81">
   <si>
     <t>Fecha</t>
   </si>
@@ -193,15 +193,94 @@
   <si>
     <t>Bote</t>
   </si>
+  <si>
+    <t>Resistencia Aerobica</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A.F.G    </t>
+  </si>
+  <si>
+    <t>A.F.G. 1</t>
+  </si>
+  <si>
+    <t>(10' + 6' + 10' ) -&gt; 26'</t>
+  </si>
+  <si>
+    <t>Flexiones</t>
+  </si>
+  <si>
+    <t>Abdominales en el suelo con las rodillas flexionadas.</t>
+  </si>
+  <si>
+    <t>Lanzamientos de balon medicinal (al suelo)</t>
+  </si>
+  <si>
+    <t>Extensiones de espalda</t>
+  </si>
+  <si>
+    <t>Saltos en zig-zag por encima de los bancos.</t>
+  </si>
+  <si>
+    <t>Triceps</t>
+  </si>
+  <si>
+    <t>Abdominales</t>
+  </si>
+  <si>
+    <t>Lanzamientos de balon medicinal (al pecho del compañero)</t>
+  </si>
+  <si>
+    <t>Lumbares</t>
+  </si>
+  <si>
+    <t>Saltar sobre el banco y al suelo</t>
+  </si>
+  <si>
+    <t>Trabajo</t>
+  </si>
+  <si>
+    <t>Por parejas</t>
+  </si>
+  <si>
+    <t>1 trabaja y el otro descansa</t>
+  </si>
+  <si>
+    <t>30' trabajo + 30' recuperacion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Material </t>
+  </si>
+  <si>
+    <t>Balones medicinales</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bancos </t>
+  </si>
+  <si>
+    <t>Carrera continua alrededor del pista balonmano</t>
+  </si>
+  <si>
+    <t>4 x (ABD(25) + LUMB(15) + FLEXIONES(15) + SALTOS(15) )</t>
+  </si>
+  <si>
+    <t>Calentamiento: (15')</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="6">
+  <fonts count="10">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="14"/>
@@ -231,8 +310,29 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -251,8 +351,47 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="13">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -392,169 +531,356 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="dotted">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="dotted">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="dotted">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="dotted">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="dotted">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="dotted">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="118">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="5" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="6" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -566,65 +892,120 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="17" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="18" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="19" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="4" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="5"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="6" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="6" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="20" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="21" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="22" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="7">
+    <cellStyle name="20% - Énfasis1" xfId="2" builtinId="30"/>
+    <cellStyle name="20% - Énfasis2" xfId="4" builtinId="34"/>
+    <cellStyle name="20% - Énfasis4" xfId="6" builtinId="42"/>
+    <cellStyle name="Énfasis1" xfId="1" builtinId="29"/>
+    <cellStyle name="Énfasis2" xfId="3" builtinId="33"/>
+    <cellStyle name="Énfasis4" xfId="5" builtinId="41"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -9588,33 +9969,36 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:W98"/>
+  <dimension ref="A1:W83"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="M20" sqref="M20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19:I35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="18"/>
   <cols>
-    <col min="1" max="22" width="9.140625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="5.42578125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="2" hidden="1" customWidth="1"/>
+    <col min="4" max="22" width="9.140625" style="2" customWidth="1"/>
     <col min="23" max="23" width="12.7109375" style="2" customWidth="1"/>
     <col min="24" max="16384" width="9.140625" style="1" hidden="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="55" t="s">
         <v>54</v>
       </c>
-      <c r="B1" s="48"/>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
-      <c r="F1" s="48"/>
-      <c r="G1" s="48"/>
-      <c r="H1" s="48"/>
-      <c r="I1" s="48"/>
-      <c r="J1" s="48"/>
-      <c r="K1" s="49"/>
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="56"/>
+      <c r="H1" s="56"/>
+      <c r="I1" s="56"/>
+      <c r="J1" s="56"/>
+      <c r="K1" s="57"/>
       <c r="L1" s="29"/>
       <c r="M1" s="29"/>
       <c r="N1" s="29"/>
@@ -9628,17 +10012,17 @@
       <c r="V1" s="29"/>
     </row>
     <row r="2" spans="1:23">
-      <c r="A2" s="50"/>
-      <c r="B2" s="51"/>
-      <c r="C2" s="51"/>
-      <c r="D2" s="51"/>
-      <c r="E2" s="51"/>
-      <c r="F2" s="51"/>
-      <c r="G2" s="51"/>
-      <c r="H2" s="51"/>
-      <c r="I2" s="51"/>
-      <c r="J2" s="51"/>
-      <c r="K2" s="52"/>
+      <c r="A2" s="58"/>
+      <c r="B2" s="59"/>
+      <c r="C2" s="59"/>
+      <c r="D2" s="59"/>
+      <c r="E2" s="59"/>
+      <c r="F2" s="59"/>
+      <c r="G2" s="59"/>
+      <c r="H2" s="59"/>
+      <c r="I2" s="59"/>
+      <c r="J2" s="59"/>
+      <c r="K2" s="60"/>
       <c r="L2" s="29"/>
       <c r="M2" s="29"/>
       <c r="N2" s="29"/>
@@ -9652,17 +10036,17 @@
       <c r="V2" s="29"/>
     </row>
     <row r="3" spans="1:23">
-      <c r="A3" s="31"/>
-      <c r="B3" s="31"/>
-      <c r="C3" s="31"/>
-      <c r="D3" s="31"/>
-      <c r="E3" s="31"/>
-      <c r="F3" s="31"/>
-      <c r="G3" s="31"/>
-      <c r="H3" s="31"/>
-      <c r="I3" s="31"/>
-      <c r="J3" s="31"/>
-      <c r="K3" s="31"/>
+      <c r="A3" s="64"/>
+      <c r="B3" s="64"/>
+      <c r="C3" s="64"/>
+      <c r="D3" s="64"/>
+      <c r="E3" s="64"/>
+      <c r="F3" s="64"/>
+      <c r="G3" s="64"/>
+      <c r="H3" s="64"/>
+      <c r="I3" s="64"/>
+      <c r="J3" s="64"/>
+      <c r="K3" s="64"/>
       <c r="L3" s="29"/>
       <c r="M3" s="29"/>
       <c r="N3" s="29"/>
@@ -9676,29 +10060,29 @@
       <c r="V3" s="29"/>
     </row>
     <row r="4" spans="1:23">
-      <c r="A4" s="38" t="s">
+      <c r="A4" s="35" t="s">
         <v>35</v>
       </c>
-      <c r="B4" s="40"/>
-      <c r="C4" s="39"/>
-      <c r="D4" s="38" t="s">
+      <c r="B4" s="36"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="39"/>
+      <c r="E4" s="37"/>
       <c r="F4" s="26">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G4" s="21" t="s">
         <v>0</v>
       </c>
       <c r="H4" s="27">
-        <v>40778</v>
+        <v>40773</v>
       </c>
-      <c r="I4" s="38" t="s">
+      <c r="I4" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="J4" s="40"/>
-      <c r="K4" s="39"/>
+      <c r="J4" s="36"/>
+      <c r="K4" s="37"/>
       <c r="L4" s="30"/>
       <c r="M4" s="30"/>
       <c r="N4" s="30"/>
@@ -9712,19 +10096,2235 @@
       <c r="V4" s="30"/>
     </row>
     <row r="5" spans="1:23" ht="18" customHeight="1">
-      <c r="A5" s="35"/>
-      <c r="B5" s="36"/>
-      <c r="C5" s="37"/>
-      <c r="D5" s="38" t="s">
+      <c r="A5" s="65"/>
+      <c r="B5" s="66"/>
+      <c r="C5" s="67"/>
+      <c r="D5" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="E5" s="40"/>
-      <c r="F5" s="40"/>
-      <c r="G5" s="40"/>
-      <c r="H5" s="39"/>
-      <c r="I5" s="67"/>
-      <c r="J5" s="68"/>
-      <c r="K5" s="69"/>
+      <c r="E5" s="36"/>
+      <c r="F5" s="36"/>
+      <c r="G5" s="36"/>
+      <c r="H5" s="37"/>
+      <c r="I5" s="68"/>
+      <c r="J5" s="69"/>
+      <c r="K5" s="70"/>
+      <c r="L5" s="31"/>
+      <c r="M5" s="31"/>
+      <c r="N5" s="31"/>
+      <c r="O5" s="31"/>
+      <c r="P5" s="31"/>
+      <c r="Q5" s="31"/>
+      <c r="R5" s="31"/>
+      <c r="S5" s="31"/>
+      <c r="T5" s="31"/>
+      <c r="U5" s="31"/>
+      <c r="V5" s="31"/>
+    </row>
+    <row r="6" spans="1:23" ht="18" customHeight="1">
+      <c r="A6" s="35" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="36"/>
+      <c r="C6" s="37"/>
+      <c r="D6" s="46" t="s">
+        <v>58</v>
+      </c>
+      <c r="E6" s="47"/>
+      <c r="F6" s="47"/>
+      <c r="G6" s="47"/>
+      <c r="H6" s="48"/>
+      <c r="I6" s="43"/>
+      <c r="J6" s="44"/>
+      <c r="K6" s="45"/>
+      <c r="L6" s="31"/>
+      <c r="M6" s="31"/>
+      <c r="N6" s="31"/>
+      <c r="O6" s="31"/>
+      <c r="P6" s="31"/>
+      <c r="Q6" s="31"/>
+      <c r="R6" s="31"/>
+      <c r="S6" s="31"/>
+      <c r="T6" s="31"/>
+      <c r="U6" s="31"/>
+      <c r="V6" s="31"/>
+    </row>
+    <row r="7" spans="1:23">
+      <c r="A7" s="46"/>
+      <c r="B7" s="47"/>
+      <c r="C7" s="48"/>
+      <c r="D7" s="49" t="s">
+        <v>57</v>
+      </c>
+      <c r="E7" s="50"/>
+      <c r="F7" s="50"/>
+      <c r="G7" s="50"/>
+      <c r="H7" s="51"/>
+      <c r="I7" s="43"/>
+      <c r="J7" s="44"/>
+      <c r="K7" s="45"/>
+      <c r="L7" s="31"/>
+      <c r="M7" s="31"/>
+      <c r="N7" s="31"/>
+      <c r="O7" s="31"/>
+      <c r="P7" s="31"/>
+      <c r="Q7" s="31"/>
+      <c r="R7" s="31"/>
+      <c r="S7" s="31"/>
+      <c r="T7" s="31"/>
+      <c r="U7" s="31"/>
+      <c r="V7" s="31"/>
+    </row>
+    <row r="8" spans="1:23">
+      <c r="A8" s="49"/>
+      <c r="B8" s="50"/>
+      <c r="C8" s="51"/>
+      <c r="D8" s="35" t="s">
+        <v>38</v>
+      </c>
+      <c r="E8" s="36"/>
+      <c r="F8" s="36"/>
+      <c r="G8" s="36"/>
+      <c r="H8" s="37"/>
+      <c r="I8" s="43"/>
+      <c r="J8" s="44"/>
+      <c r="K8" s="45"/>
+      <c r="L8" s="31"/>
+      <c r="M8" s="31"/>
+      <c r="N8" s="31"/>
+      <c r="O8" s="31"/>
+      <c r="P8" s="31"/>
+      <c r="Q8" s="31"/>
+      <c r="R8" s="31"/>
+      <c r="S8" s="31"/>
+      <c r="T8" s="31"/>
+      <c r="U8" s="31"/>
+      <c r="V8" s="31"/>
+    </row>
+    <row r="9" spans="1:23">
+      <c r="A9" s="35" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="36"/>
+      <c r="C9" s="37"/>
+      <c r="D9" s="65"/>
+      <c r="E9" s="66"/>
+      <c r="F9" s="66"/>
+      <c r="G9" s="66"/>
+      <c r="H9" s="67"/>
+      <c r="I9" s="43"/>
+      <c r="J9" s="44"/>
+      <c r="K9" s="45"/>
+      <c r="L9" s="31"/>
+      <c r="M9" s="31"/>
+      <c r="N9" s="31"/>
+      <c r="O9" s="31"/>
+      <c r="P9" s="31"/>
+      <c r="Q9" s="31"/>
+      <c r="R9" s="31"/>
+      <c r="S9" s="31"/>
+      <c r="T9" s="31"/>
+      <c r="U9" s="31"/>
+      <c r="V9" s="31"/>
+    </row>
+    <row r="10" spans="1:23">
+      <c r="A10" s="46"/>
+      <c r="B10" s="47"/>
+      <c r="C10" s="48"/>
+      <c r="D10" s="35" t="s">
+        <v>36</v>
+      </c>
+      <c r="E10" s="36"/>
+      <c r="F10" s="36"/>
+      <c r="G10" s="36"/>
+      <c r="H10" s="37"/>
+      <c r="I10" s="43"/>
+      <c r="J10" s="44"/>
+      <c r="K10" s="45"/>
+      <c r="L10" s="31"/>
+      <c r="M10" s="31"/>
+      <c r="N10" s="31"/>
+      <c r="O10" s="31"/>
+      <c r="P10" s="31"/>
+      <c r="Q10" s="31"/>
+      <c r="R10" s="31"/>
+      <c r="S10" s="31"/>
+      <c r="T10" s="31"/>
+      <c r="U10" s="31"/>
+      <c r="V10" s="31"/>
+    </row>
+    <row r="11" spans="1:23">
+      <c r="A11" s="49"/>
+      <c r="B11" s="50"/>
+      <c r="C11" s="51"/>
+      <c r="D11" s="61"/>
+      <c r="E11" s="62"/>
+      <c r="F11" s="62"/>
+      <c r="G11" s="62"/>
+      <c r="H11" s="63"/>
+      <c r="I11" s="52"/>
+      <c r="J11" s="53"/>
+      <c r="K11" s="54"/>
+      <c r="L11" s="31"/>
+      <c r="M11" s="31"/>
+      <c r="N11" s="31"/>
+      <c r="O11" s="31"/>
+      <c r="P11" s="31"/>
+      <c r="Q11" s="31"/>
+      <c r="R11" s="31"/>
+      <c r="S11" s="31"/>
+      <c r="T11" s="31"/>
+      <c r="U11" s="31"/>
+      <c r="V11" s="31"/>
+    </row>
+    <row r="12" spans="1:23">
+      <c r="A12" s="32"/>
+      <c r="B12" s="32"/>
+      <c r="C12" s="32"/>
+      <c r="D12" s="33"/>
+      <c r="E12" s="33"/>
+      <c r="F12" s="33"/>
+      <c r="G12" s="33"/>
+      <c r="H12" s="33"/>
+      <c r="I12" s="34"/>
+      <c r="J12" s="34"/>
+      <c r="K12" s="34"/>
+      <c r="L12" s="31"/>
+      <c r="M12" s="31"/>
+      <c r="N12" s="31"/>
+      <c r="O12" s="31"/>
+      <c r="P12" s="31"/>
+      <c r="Q12" s="31"/>
+      <c r="R12" s="31"/>
+      <c r="S12" s="31"/>
+      <c r="T12" s="31"/>
+      <c r="U12" s="31"/>
+      <c r="V12" s="31"/>
+    </row>
+    <row r="13" spans="1:23">
+      <c r="A13" s="62" t="s">
+        <v>80</v>
+      </c>
+      <c r="B13" s="62"/>
+      <c r="C13" s="62"/>
+      <c r="D13" s="62"/>
+      <c r="E13" s="62"/>
+      <c r="F13" s="62"/>
+      <c r="G13" s="62"/>
+      <c r="H13" s="62"/>
+      <c r="I13" s="62"/>
+      <c r="J13" s="62"/>
+      <c r="K13" s="62"/>
+      <c r="L13" s="31"/>
+      <c r="M13" s="31"/>
+      <c r="N13" s="31"/>
+      <c r="O13" s="31"/>
+      <c r="P13" s="31"/>
+      <c r="Q13" s="31"/>
+      <c r="R13" s="31"/>
+      <c r="S13" s="31"/>
+      <c r="T13" s="31"/>
+      <c r="U13" s="31"/>
+      <c r="V13" s="31"/>
+    </row>
+    <row r="14" spans="1:23" s="110" customFormat="1" ht="15">
+      <c r="A14" s="112" t="s">
+        <v>78</v>
+      </c>
+      <c r="B14" s="112"/>
+      <c r="C14" s="112"/>
+      <c r="D14" s="112"/>
+      <c r="E14" s="112"/>
+      <c r="F14" s="112"/>
+      <c r="G14" s="112"/>
+      <c r="H14" s="112"/>
+      <c r="I14" s="112"/>
+      <c r="J14" s="112"/>
+      <c r="K14" s="112"/>
+      <c r="L14" s="108"/>
+      <c r="M14" s="108"/>
+      <c r="N14" s="108"/>
+      <c r="O14" s="108"/>
+      <c r="P14" s="108"/>
+      <c r="Q14" s="108"/>
+      <c r="R14" s="108"/>
+      <c r="S14" s="108"/>
+      <c r="T14" s="108"/>
+      <c r="U14" s="108"/>
+      <c r="V14" s="108"/>
+      <c r="W14" s="109"/>
+    </row>
+    <row r="15" spans="1:23" s="110" customFormat="1" ht="15">
+      <c r="A15" s="112" t="s">
+        <v>79</v>
+      </c>
+      <c r="B15" s="112"/>
+      <c r="C15" s="112"/>
+      <c r="D15" s="112"/>
+      <c r="E15" s="112"/>
+      <c r="F15" s="112"/>
+      <c r="G15" s="112"/>
+      <c r="H15" s="112"/>
+      <c r="I15" s="112"/>
+      <c r="J15" s="112"/>
+      <c r="K15" s="112"/>
+      <c r="L15" s="111"/>
+      <c r="M15" s="111"/>
+      <c r="N15" s="111"/>
+      <c r="O15" s="111"/>
+      <c r="P15" s="111"/>
+      <c r="Q15" s="111"/>
+      <c r="R15" s="111"/>
+      <c r="S15" s="111"/>
+      <c r="T15" s="111"/>
+      <c r="U15" s="111"/>
+      <c r="V15" s="111"/>
+      <c r="W15" s="109"/>
+    </row>
+    <row r="16" spans="1:23" s="110" customFormat="1" ht="15">
+      <c r="A16" s="113"/>
+      <c r="B16" s="113"/>
+      <c r="C16" s="113"/>
+      <c r="D16" s="113"/>
+      <c r="E16" s="113"/>
+      <c r="F16" s="113"/>
+      <c r="G16" s="113"/>
+      <c r="H16" s="113"/>
+      <c r="I16" s="113"/>
+      <c r="J16" s="113"/>
+      <c r="K16" s="113"/>
+      <c r="L16" s="111"/>
+      <c r="M16" s="111"/>
+      <c r="N16" s="111"/>
+      <c r="O16" s="111"/>
+      <c r="P16" s="111"/>
+      <c r="Q16" s="111"/>
+      <c r="R16" s="111"/>
+      <c r="S16" s="111"/>
+      <c r="T16" s="111"/>
+      <c r="U16" s="111"/>
+      <c r="V16" s="111"/>
+      <c r="W16" s="109"/>
+    </row>
+    <row r="17" spans="1:23" ht="18" customHeight="1">
+      <c r="A17" s="35" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" s="36"/>
+      <c r="C17" s="36"/>
+      <c r="D17" s="36"/>
+      <c r="E17" s="36"/>
+      <c r="F17" s="36"/>
+      <c r="G17" s="36"/>
+      <c r="H17" s="36"/>
+      <c r="I17" s="36"/>
+      <c r="J17" s="36"/>
+      <c r="K17" s="37"/>
+      <c r="L17" s="35" t="s">
+        <v>6</v>
+      </c>
+      <c r="M17" s="36"/>
+      <c r="N17" s="36"/>
+      <c r="O17" s="36"/>
+      <c r="P17" s="36"/>
+      <c r="Q17" s="36"/>
+      <c r="R17" s="36"/>
+      <c r="S17" s="36"/>
+      <c r="T17" s="36"/>
+      <c r="U17" s="36"/>
+      <c r="V17" s="37"/>
+    </row>
+    <row r="18" spans="1:23" s="4" customFormat="1" ht="12.75">
+      <c r="A18" s="13"/>
+      <c r="B18" s="14"/>
+      <c r="C18" s="14"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="14"/>
+      <c r="G18" s="14"/>
+      <c r="H18" s="14"/>
+      <c r="I18" s="14"/>
+      <c r="J18" s="14"/>
+      <c r="K18" s="15"/>
+      <c r="L18" s="13"/>
+      <c r="M18" s="14"/>
+      <c r="N18" s="14"/>
+      <c r="O18" s="14"/>
+      <c r="P18" s="14"/>
+      <c r="Q18" s="14"/>
+      <c r="R18" s="14"/>
+      <c r="S18" s="14"/>
+      <c r="T18" s="14"/>
+      <c r="U18" s="14"/>
+      <c r="V18" s="15"/>
+      <c r="W18" s="3"/>
+    </row>
+    <row r="19" spans="1:23" s="4" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A19" s="13"/>
+      <c r="B19" s="14"/>
+      <c r="C19" s="14"/>
+      <c r="D19" s="87" t="s">
+        <v>59</v>
+      </c>
+      <c r="E19" s="114" t="s">
+        <v>60</v>
+      </c>
+      <c r="F19" s="114"/>
+      <c r="G19" s="114"/>
+      <c r="H19" s="114"/>
+      <c r="I19" s="88"/>
+      <c r="J19" s="14"/>
+      <c r="K19" s="15"/>
+      <c r="L19" s="13"/>
+      <c r="M19" s="14"/>
+      <c r="N19" s="14"/>
+      <c r="O19" s="14"/>
+      <c r="P19" s="14"/>
+      <c r="Q19" s="14"/>
+      <c r="R19" s="14"/>
+      <c r="S19" s="14"/>
+      <c r="T19" s="14"/>
+      <c r="U19" s="14"/>
+      <c r="V19" s="15"/>
+      <c r="W19" s="3"/>
+    </row>
+    <row r="20" spans="1:23" s="4" customFormat="1" ht="15" customHeight="1">
+      <c r="A20" s="13"/>
+      <c r="B20" s="14"/>
+      <c r="C20" s="14"/>
+      <c r="D20" s="89" t="s">
+        <v>61</v>
+      </c>
+      <c r="E20" s="90"/>
+      <c r="F20" s="90"/>
+      <c r="G20" s="90"/>
+      <c r="H20" s="90"/>
+      <c r="I20" s="91"/>
+      <c r="J20" s="14"/>
+      <c r="K20" s="15"/>
+      <c r="L20" s="13"/>
+      <c r="M20" s="14"/>
+      <c r="N20" s="14"/>
+      <c r="O20" s="14"/>
+      <c r="P20" s="14"/>
+      <c r="Q20" s="14"/>
+      <c r="R20" s="14"/>
+      <c r="S20" s="14"/>
+      <c r="T20" s="14"/>
+      <c r="U20" s="14"/>
+      <c r="V20" s="15"/>
+      <c r="W20" s="3"/>
+    </row>
+    <row r="21" spans="1:23" s="4" customFormat="1" ht="15" customHeight="1">
+      <c r="A21" s="13"/>
+      <c r="B21" s="14"/>
+      <c r="C21" s="14"/>
+      <c r="D21" s="92" t="s">
+        <v>62</v>
+      </c>
+      <c r="E21" s="93"/>
+      <c r="F21" s="93"/>
+      <c r="G21" s="93"/>
+      <c r="H21" s="93"/>
+      <c r="I21" s="94"/>
+      <c r="J21" s="14"/>
+      <c r="K21" s="15"/>
+      <c r="L21" s="13"/>
+      <c r="M21" s="14"/>
+      <c r="N21" s="14"/>
+      <c r="O21" s="14"/>
+      <c r="P21" s="14"/>
+      <c r="Q21" s="14"/>
+      <c r="R21" s="14"/>
+      <c r="S21" s="14"/>
+      <c r="T21" s="14"/>
+      <c r="U21" s="14"/>
+      <c r="V21" s="15"/>
+      <c r="W21" s="3"/>
+    </row>
+    <row r="22" spans="1:23" s="4" customFormat="1" ht="15" customHeight="1">
+      <c r="A22" s="13"/>
+      <c r="B22" s="14"/>
+      <c r="C22" s="14"/>
+      <c r="D22" s="92" t="s">
+        <v>63</v>
+      </c>
+      <c r="E22" s="93"/>
+      <c r="F22" s="93"/>
+      <c r="G22" s="93"/>
+      <c r="H22" s="93"/>
+      <c r="I22" s="94"/>
+      <c r="J22" s="14"/>
+      <c r="K22" s="15"/>
+      <c r="L22" s="13"/>
+      <c r="M22" s="14"/>
+      <c r="N22" s="14"/>
+      <c r="O22" s="14"/>
+      <c r="P22" s="14"/>
+      <c r="Q22" s="14"/>
+      <c r="R22" s="14"/>
+      <c r="S22" s="14"/>
+      <c r="T22" s="14"/>
+      <c r="U22" s="14"/>
+      <c r="V22" s="15"/>
+      <c r="W22" s="3"/>
+    </row>
+    <row r="23" spans="1:23" s="4" customFormat="1" ht="15" customHeight="1">
+      <c r="A23" s="13"/>
+      <c r="B23" s="14"/>
+      <c r="C23" s="14"/>
+      <c r="D23" s="92" t="s">
+        <v>64</v>
+      </c>
+      <c r="E23" s="93"/>
+      <c r="F23" s="93"/>
+      <c r="G23" s="93"/>
+      <c r="H23" s="93"/>
+      <c r="I23" s="94"/>
+      <c r="J23" s="14"/>
+      <c r="K23" s="15"/>
+      <c r="L23" s="13"/>
+      <c r="M23" s="14"/>
+      <c r="N23" s="14"/>
+      <c r="O23" s="14"/>
+      <c r="P23" s="14"/>
+      <c r="Q23" s="14"/>
+      <c r="R23" s="14"/>
+      <c r="S23" s="14"/>
+      <c r="T23" s="14"/>
+      <c r="U23" s="14"/>
+      <c r="V23" s="15"/>
+      <c r="W23" s="3"/>
+    </row>
+    <row r="24" spans="1:23" s="4" customFormat="1" ht="15" customHeight="1">
+      <c r="A24" s="16"/>
+      <c r="B24" s="14"/>
+      <c r="C24" s="14"/>
+      <c r="D24" s="95" t="s">
+        <v>65</v>
+      </c>
+      <c r="E24" s="96"/>
+      <c r="F24" s="96"/>
+      <c r="G24" s="96"/>
+      <c r="H24" s="96"/>
+      <c r="I24" s="97"/>
+      <c r="J24" s="14"/>
+      <c r="K24" s="15"/>
+      <c r="L24" s="16"/>
+      <c r="M24" s="14"/>
+      <c r="N24" s="14"/>
+      <c r="O24" s="14"/>
+      <c r="P24" s="14"/>
+      <c r="Q24" s="20"/>
+      <c r="R24" s="14"/>
+      <c r="S24" s="14"/>
+      <c r="T24" s="14"/>
+      <c r="U24" s="14"/>
+      <c r="V24" s="15"/>
+      <c r="W24" s="3"/>
+    </row>
+    <row r="25" spans="1:23" s="4" customFormat="1" ht="15" customHeight="1">
+      <c r="A25" s="13"/>
+      <c r="B25" s="14"/>
+      <c r="C25" s="14"/>
+      <c r="D25" s="115" t="s">
+        <v>66</v>
+      </c>
+      <c r="E25" s="116"/>
+      <c r="F25" s="116"/>
+      <c r="G25" s="116"/>
+      <c r="H25" s="116"/>
+      <c r="I25" s="117"/>
+      <c r="J25" s="14"/>
+      <c r="K25" s="15"/>
+      <c r="L25" s="13"/>
+      <c r="M25" s="14"/>
+      <c r="N25" s="14"/>
+      <c r="O25" s="14"/>
+      <c r="P25" s="14"/>
+      <c r="Q25" s="14"/>
+      <c r="R25" s="14"/>
+      <c r="S25" s="14"/>
+      <c r="T25" s="14"/>
+      <c r="U25" s="14"/>
+      <c r="V25" s="15"/>
+      <c r="W25" s="3"/>
+    </row>
+    <row r="26" spans="1:23" s="4" customFormat="1" ht="15" customHeight="1">
+      <c r="A26" s="13"/>
+      <c r="B26" s="14"/>
+      <c r="C26" s="14"/>
+      <c r="D26" s="92" t="s">
+        <v>67</v>
+      </c>
+      <c r="E26" s="93"/>
+      <c r="F26" s="93"/>
+      <c r="G26" s="93"/>
+      <c r="H26" s="93"/>
+      <c r="I26" s="94"/>
+      <c r="J26" s="14"/>
+      <c r="K26" s="15"/>
+      <c r="L26" s="13"/>
+      <c r="M26" s="14"/>
+      <c r="N26" s="14"/>
+      <c r="O26" s="14"/>
+      <c r="P26" s="14"/>
+      <c r="Q26" s="14"/>
+      <c r="R26" s="14"/>
+      <c r="S26" s="14"/>
+      <c r="T26" s="14"/>
+      <c r="U26" s="14"/>
+      <c r="V26" s="15"/>
+      <c r="W26" s="3"/>
+    </row>
+    <row r="27" spans="1:23" s="4" customFormat="1" ht="15" customHeight="1">
+      <c r="A27" s="13"/>
+      <c r="B27" s="14"/>
+      <c r="C27" s="14"/>
+      <c r="D27" s="92" t="s">
+        <v>68</v>
+      </c>
+      <c r="E27" s="93"/>
+      <c r="F27" s="93"/>
+      <c r="G27" s="93"/>
+      <c r="H27" s="93"/>
+      <c r="I27" s="94"/>
+      <c r="J27" s="14"/>
+      <c r="K27" s="15"/>
+      <c r="L27" s="13"/>
+      <c r="M27" s="14"/>
+      <c r="N27" s="14"/>
+      <c r="O27" s="14"/>
+      <c r="P27" s="14"/>
+      <c r="Q27" s="14"/>
+      <c r="R27" s="14"/>
+      <c r="S27" s="14"/>
+      <c r="T27" s="14"/>
+      <c r="U27" s="14"/>
+      <c r="V27" s="15"/>
+      <c r="W27" s="3"/>
+    </row>
+    <row r="28" spans="1:23" s="4" customFormat="1" ht="15" customHeight="1">
+      <c r="A28" s="13"/>
+      <c r="B28" s="14"/>
+      <c r="C28" s="14"/>
+      <c r="D28" s="92" t="s">
+        <v>69</v>
+      </c>
+      <c r="E28" s="93"/>
+      <c r="F28" s="93"/>
+      <c r="G28" s="93"/>
+      <c r="H28" s="93"/>
+      <c r="I28" s="94"/>
+      <c r="J28" s="14"/>
+      <c r="K28" s="15"/>
+      <c r="L28" s="13"/>
+      <c r="M28" s="14"/>
+      <c r="N28" s="14"/>
+      <c r="O28" s="14"/>
+      <c r="P28" s="14"/>
+      <c r="Q28" s="14"/>
+      <c r="R28" s="14"/>
+      <c r="S28" s="14"/>
+      <c r="T28" s="14"/>
+      <c r="U28" s="14"/>
+      <c r="V28" s="15"/>
+      <c r="W28" s="3"/>
+    </row>
+    <row r="29" spans="1:23" s="4" customFormat="1" ht="15" customHeight="1">
+      <c r="A29" s="13"/>
+      <c r="B29" s="14"/>
+      <c r="C29" s="14"/>
+      <c r="D29" s="98" t="s">
+        <v>70</v>
+      </c>
+      <c r="E29" s="99"/>
+      <c r="F29" s="99"/>
+      <c r="G29" s="99"/>
+      <c r="H29" s="99"/>
+      <c r="I29" s="100"/>
+      <c r="J29" s="14"/>
+      <c r="K29" s="15"/>
+      <c r="L29" s="13"/>
+      <c r="M29" s="14"/>
+      <c r="N29" s="14"/>
+      <c r="O29" s="14"/>
+      <c r="P29" s="14"/>
+      <c r="Q29" s="14"/>
+      <c r="R29" s="14"/>
+      <c r="S29" s="14"/>
+      <c r="T29" s="14"/>
+      <c r="U29" s="14"/>
+      <c r="V29" s="15"/>
+      <c r="W29" s="3"/>
+    </row>
+    <row r="30" spans="1:23" s="4" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A30" s="13"/>
+      <c r="B30" s="14"/>
+      <c r="C30" s="14"/>
+      <c r="D30"/>
+      <c r="E30"/>
+      <c r="F30"/>
+      <c r="G30"/>
+      <c r="H30"/>
+      <c r="I30"/>
+      <c r="J30" s="14"/>
+      <c r="K30" s="15"/>
+      <c r="L30" s="13"/>
+      <c r="M30" s="14"/>
+      <c r="N30" s="14"/>
+      <c r="O30" s="14"/>
+      <c r="P30" s="14"/>
+      <c r="Q30" s="14"/>
+      <c r="R30" s="14"/>
+      <c r="S30" s="14"/>
+      <c r="T30" s="14"/>
+      <c r="U30" s="14"/>
+      <c r="V30" s="15"/>
+      <c r="W30" s="3"/>
+    </row>
+    <row r="31" spans="1:23" s="4" customFormat="1" ht="15" customHeight="1">
+      <c r="A31" s="13"/>
+      <c r="B31" s="14"/>
+      <c r="C31" s="14"/>
+      <c r="D31" s="101" t="s">
+        <v>71</v>
+      </c>
+      <c r="E31" s="102" t="s">
+        <v>72</v>
+      </c>
+      <c r="F31" s="103" t="s">
+        <v>73</v>
+      </c>
+      <c r="G31" s="103"/>
+      <c r="H31" s="103"/>
+      <c r="I31"/>
+      <c r="J31" s="14"/>
+      <c r="K31" s="15"/>
+      <c r="L31" s="13"/>
+      <c r="M31" s="14"/>
+      <c r="N31" s="14"/>
+      <c r="O31" s="14"/>
+      <c r="P31" s="14"/>
+      <c r="Q31" s="14"/>
+      <c r="R31" s="14"/>
+      <c r="S31" s="14"/>
+      <c r="T31" s="14"/>
+      <c r="U31" s="14"/>
+      <c r="V31" s="15"/>
+      <c r="W31" s="3"/>
+    </row>
+    <row r="32" spans="1:23" s="4" customFormat="1" ht="15" customHeight="1">
+      <c r="A32" s="13"/>
+      <c r="B32" s="14"/>
+      <c r="C32" s="14"/>
+      <c r="D32" s="101"/>
+      <c r="E32" s="102"/>
+      <c r="F32" s="104" t="s">
+        <v>74</v>
+      </c>
+      <c r="G32" s="104"/>
+      <c r="H32" s="104"/>
+      <c r="I32"/>
+      <c r="J32" s="14"/>
+      <c r="K32" s="15"/>
+      <c r="L32" s="13"/>
+      <c r="M32" s="14"/>
+      <c r="N32" s="14"/>
+      <c r="O32" s="14"/>
+      <c r="P32" s="14"/>
+      <c r="Q32" s="14"/>
+      <c r="R32" s="14"/>
+      <c r="S32" s="14"/>
+      <c r="T32" s="14"/>
+      <c r="U32" s="14"/>
+      <c r="V32" s="15"/>
+      <c r="W32" s="3"/>
+    </row>
+    <row r="33" spans="1:23" s="4" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A33" s="13"/>
+      <c r="B33" s="14"/>
+      <c r="C33" s="14"/>
+      <c r="D33"/>
+      <c r="E33"/>
+      <c r="F33"/>
+      <c r="G33"/>
+      <c r="H33"/>
+      <c r="I33"/>
+      <c r="J33" s="14"/>
+      <c r="K33" s="15"/>
+      <c r="L33" s="13"/>
+      <c r="M33" s="14"/>
+      <c r="N33" s="14"/>
+      <c r="O33" s="14"/>
+      <c r="P33" s="14"/>
+      <c r="Q33" s="14"/>
+      <c r="R33" s="14"/>
+      <c r="S33" s="14"/>
+      <c r="T33" s="14"/>
+      <c r="U33" s="14"/>
+      <c r="V33" s="15"/>
+      <c r="W33" s="3"/>
+    </row>
+    <row r="34" spans="1:23" s="4" customFormat="1" ht="15" customHeight="1">
+      <c r="A34" s="13"/>
+      <c r="B34" s="14"/>
+      <c r="C34" s="14"/>
+      <c r="D34" s="105" t="s">
+        <v>75</v>
+      </c>
+      <c r="E34" s="106" t="s">
+        <v>76</v>
+      </c>
+      <c r="F34" s="106"/>
+      <c r="G34" s="107">
+        <v>2</v>
+      </c>
+      <c r="H34"/>
+      <c r="I34"/>
+      <c r="J34" s="14"/>
+      <c r="K34" s="15"/>
+      <c r="L34" s="13"/>
+      <c r="M34" s="14"/>
+      <c r="N34" s="14"/>
+      <c r="O34" s="14"/>
+      <c r="P34" s="14"/>
+      <c r="Q34" s="14"/>
+      <c r="R34" s="14"/>
+      <c r="S34" s="14"/>
+      <c r="T34" s="14"/>
+      <c r="U34" s="14"/>
+      <c r="V34" s="15"/>
+      <c r="W34" s="3"/>
+    </row>
+    <row r="35" spans="1:23" s="4" customFormat="1" ht="15" customHeight="1">
+      <c r="A35" s="13"/>
+      <c r="B35" s="14"/>
+      <c r="C35" s="14"/>
+      <c r="D35" s="105"/>
+      <c r="E35" s="106" t="s">
+        <v>77</v>
+      </c>
+      <c r="F35" s="106"/>
+      <c r="G35" s="107">
+        <v>1</v>
+      </c>
+      <c r="H35"/>
+      <c r="I35"/>
+      <c r="J35" s="14"/>
+      <c r="K35" s="15"/>
+      <c r="L35" s="13"/>
+      <c r="M35" s="14"/>
+      <c r="N35" s="14"/>
+      <c r="O35" s="14"/>
+      <c r="P35" s="14"/>
+      <c r="Q35" s="14"/>
+      <c r="R35" s="14"/>
+      <c r="S35" s="14"/>
+      <c r="T35" s="14"/>
+      <c r="U35" s="14"/>
+      <c r="V35" s="15"/>
+      <c r="W35" s="3"/>
+    </row>
+    <row r="36" spans="1:23" s="4" customFormat="1" ht="12.75">
+      <c r="A36" s="13"/>
+      <c r="B36" s="14"/>
+      <c r="C36" s="14"/>
+      <c r="D36" s="14"/>
+      <c r="E36" s="14"/>
+      <c r="F36" s="14"/>
+      <c r="G36" s="14"/>
+      <c r="H36" s="14"/>
+      <c r="I36" s="14"/>
+      <c r="J36" s="14"/>
+      <c r="K36" s="15"/>
+      <c r="L36" s="13"/>
+      <c r="M36" s="14"/>
+      <c r="N36" s="14"/>
+      <c r="O36" s="14"/>
+      <c r="P36" s="14"/>
+      <c r="Q36" s="14"/>
+      <c r="R36" s="14"/>
+      <c r="S36" s="14"/>
+      <c r="T36" s="14"/>
+      <c r="U36" s="14"/>
+      <c r="V36" s="15"/>
+      <c r="W36" s="3"/>
+    </row>
+    <row r="37" spans="1:23">
+      <c r="A37" s="38" t="s">
+        <v>1</v>
+      </c>
+      <c r="B37" s="39"/>
+      <c r="C37" s="39"/>
+      <c r="D37" s="39"/>
+      <c r="E37" s="39"/>
+      <c r="F37" s="39"/>
+      <c r="G37" s="39"/>
+      <c r="H37" s="39"/>
+      <c r="I37" s="39"/>
+      <c r="J37" s="39"/>
+      <c r="K37" s="40"/>
+      <c r="L37" s="38" t="s">
+        <v>1</v>
+      </c>
+      <c r="M37" s="39"/>
+      <c r="N37" s="39"/>
+      <c r="O37" s="39"/>
+      <c r="P37" s="39"/>
+      <c r="Q37" s="39"/>
+      <c r="R37" s="39"/>
+      <c r="S37" s="39"/>
+      <c r="T37" s="39"/>
+      <c r="U37" s="39"/>
+      <c r="V37" s="40"/>
+    </row>
+    <row r="38" spans="1:23">
+      <c r="A38" s="24"/>
+      <c r="B38" s="5"/>
+      <c r="C38" s="5"/>
+      <c r="D38" s="5"/>
+      <c r="E38" s="5"/>
+      <c r="F38" s="5"/>
+      <c r="G38" s="5"/>
+      <c r="H38" s="5"/>
+      <c r="I38" s="5"/>
+      <c r="J38" s="5"/>
+      <c r="K38" s="6"/>
+      <c r="L38" s="24"/>
+      <c r="M38" s="5"/>
+      <c r="N38" s="5"/>
+      <c r="O38" s="5"/>
+      <c r="P38" s="5"/>
+      <c r="Q38" s="5"/>
+      <c r="R38" s="5"/>
+      <c r="S38" s="5"/>
+      <c r="T38" s="5"/>
+      <c r="U38" s="5"/>
+      <c r="V38" s="6"/>
+    </row>
+    <row r="39" spans="1:23">
+      <c r="A39" s="16"/>
+      <c r="B39" s="7"/>
+      <c r="C39" s="7"/>
+      <c r="D39" s="7"/>
+      <c r="E39" s="7"/>
+      <c r="F39" s="7"/>
+      <c r="G39" s="7"/>
+      <c r="H39" s="7"/>
+      <c r="I39" s="7"/>
+      <c r="J39" s="7"/>
+      <c r="K39" s="8"/>
+      <c r="L39" s="16"/>
+      <c r="M39" s="7"/>
+      <c r="N39" s="7"/>
+      <c r="O39" s="7"/>
+      <c r="P39" s="7"/>
+      <c r="Q39" s="7"/>
+      <c r="R39" s="7"/>
+      <c r="S39" s="7"/>
+      <c r="T39" s="7"/>
+      <c r="U39" s="7"/>
+      <c r="V39" s="8"/>
+    </row>
+    <row r="40" spans="1:23" ht="18.75" thickBot="1">
+      <c r="A40" s="16"/>
+      <c r="B40" s="7"/>
+      <c r="C40" s="7"/>
+      <c r="D40" s="7"/>
+      <c r="E40" s="7"/>
+      <c r="F40" s="7"/>
+      <c r="G40" s="7"/>
+      <c r="H40" s="7"/>
+      <c r="I40" s="7"/>
+      <c r="J40" s="7"/>
+      <c r="K40" s="8"/>
+      <c r="L40" s="16"/>
+      <c r="M40" s="7"/>
+      <c r="N40" s="7"/>
+      <c r="O40" s="7"/>
+      <c r="P40" s="7"/>
+      <c r="Q40" s="7"/>
+      <c r="R40" s="7"/>
+      <c r="S40" s="7"/>
+      <c r="T40" s="7"/>
+      <c r="U40" s="7"/>
+      <c r="V40" s="8"/>
+    </row>
+    <row r="41" spans="1:23" s="86" customFormat="1" ht="5.25" customHeight="1" thickBot="1">
+      <c r="A41" s="82"/>
+      <c r="B41" s="83"/>
+      <c r="C41" s="83"/>
+      <c r="D41" s="83"/>
+      <c r="E41" s="83"/>
+      <c r="F41" s="83"/>
+      <c r="G41" s="83"/>
+      <c r="H41" s="83"/>
+      <c r="I41" s="83"/>
+      <c r="J41" s="83"/>
+      <c r="K41" s="84"/>
+      <c r="L41" s="85"/>
+      <c r="M41" s="83"/>
+      <c r="N41" s="83"/>
+      <c r="O41" s="83"/>
+      <c r="P41" s="83"/>
+      <c r="Q41" s="83"/>
+      <c r="R41" s="83"/>
+      <c r="S41" s="83"/>
+      <c r="T41" s="83"/>
+      <c r="U41" s="83"/>
+      <c r="V41" s="84"/>
+    </row>
+    <row r="42" spans="1:23" ht="18" customHeight="1">
+      <c r="A42" s="80" t="s">
+        <v>6</v>
+      </c>
+      <c r="B42" s="41"/>
+      <c r="C42" s="41"/>
+      <c r="D42" s="41"/>
+      <c r="E42" s="41"/>
+      <c r="F42" s="41"/>
+      <c r="G42" s="41"/>
+      <c r="H42" s="41"/>
+      <c r="I42" s="41"/>
+      <c r="J42" s="41"/>
+      <c r="K42" s="81"/>
+      <c r="L42" s="80" t="s">
+        <v>6</v>
+      </c>
+      <c r="M42" s="41"/>
+      <c r="N42" s="41"/>
+      <c r="O42" s="41"/>
+      <c r="P42" s="41"/>
+      <c r="Q42" s="41"/>
+      <c r="R42" s="41"/>
+      <c r="S42" s="41"/>
+      <c r="T42" s="41"/>
+      <c r="U42" s="41"/>
+      <c r="V42" s="81"/>
+    </row>
+    <row r="43" spans="1:23" s="4" customFormat="1" ht="18" customHeight="1">
+      <c r="A43" s="23"/>
+      <c r="B43" s="11"/>
+      <c r="C43" s="11"/>
+      <c r="D43" s="11"/>
+      <c r="E43" s="11"/>
+      <c r="F43" s="11"/>
+      <c r="G43" s="11"/>
+      <c r="H43" s="11"/>
+      <c r="I43" s="11"/>
+      <c r="J43" s="11"/>
+      <c r="K43" s="12"/>
+      <c r="L43" s="23"/>
+      <c r="M43" s="11"/>
+      <c r="N43" s="11"/>
+      <c r="O43" s="11"/>
+      <c r="P43" s="11"/>
+      <c r="Q43" s="11"/>
+      <c r="R43" s="11"/>
+      <c r="S43" s="11"/>
+      <c r="T43" s="11"/>
+      <c r="U43" s="11"/>
+      <c r="V43" s="12"/>
+      <c r="W43" s="3"/>
+    </row>
+    <row r="44" spans="1:23" s="4" customFormat="1" ht="12.75">
+      <c r="A44" s="13"/>
+      <c r="B44" s="14"/>
+      <c r="C44" s="14"/>
+      <c r="D44" s="14"/>
+      <c r="E44" s="14"/>
+      <c r="F44" s="14"/>
+      <c r="G44" s="14"/>
+      <c r="H44" s="14"/>
+      <c r="I44" s="14"/>
+      <c r="J44" s="14"/>
+      <c r="K44" s="15"/>
+      <c r="L44" s="13"/>
+      <c r="M44" s="14"/>
+      <c r="N44" s="14"/>
+      <c r="O44" s="14"/>
+      <c r="P44" s="14"/>
+      <c r="Q44" s="14"/>
+      <c r="R44" s="14"/>
+      <c r="S44" s="14"/>
+      <c r="T44" s="14"/>
+      <c r="U44" s="14"/>
+      <c r="V44" s="15"/>
+      <c r="W44" s="3"/>
+    </row>
+    <row r="45" spans="1:23" s="4" customFormat="1" ht="12.75">
+      <c r="A45" s="13"/>
+      <c r="B45" s="14"/>
+      <c r="C45" s="14"/>
+      <c r="D45" s="14"/>
+      <c r="E45" s="14"/>
+      <c r="F45" s="14"/>
+      <c r="G45" s="14"/>
+      <c r="H45" s="14"/>
+      <c r="I45" s="14"/>
+      <c r="J45" s="14"/>
+      <c r="K45" s="15"/>
+      <c r="L45" s="13"/>
+      <c r="M45" s="14"/>
+      <c r="N45" s="14"/>
+      <c r="O45" s="14"/>
+      <c r="P45" s="14"/>
+      <c r="Q45" s="14"/>
+      <c r="R45" s="14"/>
+      <c r="S45" s="14"/>
+      <c r="T45" s="14"/>
+      <c r="U45" s="14"/>
+      <c r="V45" s="15"/>
+      <c r="W45" s="3"/>
+    </row>
+    <row r="46" spans="1:23" s="4" customFormat="1" ht="12.75">
+      <c r="A46" s="13"/>
+      <c r="B46" s="14"/>
+      <c r="C46" s="14"/>
+      <c r="D46" s="14"/>
+      <c r="E46" s="14"/>
+      <c r="F46" s="14"/>
+      <c r="G46" s="14"/>
+      <c r="H46" s="14"/>
+      <c r="I46" s="14"/>
+      <c r="J46" s="14"/>
+      <c r="K46" s="15"/>
+      <c r="L46" s="13"/>
+      <c r="M46" s="14"/>
+      <c r="N46" s="14"/>
+      <c r="O46" s="14"/>
+      <c r="P46" s="14"/>
+      <c r="Q46" s="14"/>
+      <c r="R46" s="14"/>
+      <c r="S46" s="14"/>
+      <c r="T46" s="14"/>
+      <c r="U46" s="14"/>
+      <c r="V46" s="15"/>
+      <c r="W46" s="3"/>
+    </row>
+    <row r="47" spans="1:23" s="4" customFormat="1" ht="12.75">
+      <c r="A47" s="13"/>
+      <c r="B47" s="14"/>
+      <c r="C47" s="14"/>
+      <c r="D47" s="14"/>
+      <c r="E47" s="14"/>
+      <c r="F47" s="14"/>
+      <c r="G47" s="14"/>
+      <c r="H47" s="14"/>
+      <c r="I47" s="14"/>
+      <c r="J47" s="14"/>
+      <c r="K47" s="15"/>
+      <c r="L47" s="13"/>
+      <c r="M47" s="14"/>
+      <c r="N47" s="14"/>
+      <c r="O47" s="14"/>
+      <c r="P47" s="14"/>
+      <c r="Q47" s="14"/>
+      <c r="R47" s="14"/>
+      <c r="S47" s="14"/>
+      <c r="T47" s="14"/>
+      <c r="U47" s="14"/>
+      <c r="V47" s="15"/>
+      <c r="W47" s="3"/>
+    </row>
+    <row r="48" spans="1:23" s="4" customFormat="1" ht="12.75">
+      <c r="A48" s="13"/>
+      <c r="B48" s="14"/>
+      <c r="C48" s="14"/>
+      <c r="D48" s="14"/>
+      <c r="E48" s="14"/>
+      <c r="F48" s="14"/>
+      <c r="G48" s="14"/>
+      <c r="H48" s="14"/>
+      <c r="I48" s="14"/>
+      <c r="J48" s="14"/>
+      <c r="K48" s="15"/>
+      <c r="L48" s="13"/>
+      <c r="M48" s="14"/>
+      <c r="N48" s="14"/>
+      <c r="O48" s="14"/>
+      <c r="P48" s="14"/>
+      <c r="Q48" s="14"/>
+      <c r="R48" s="14"/>
+      <c r="S48" s="14"/>
+      <c r="T48" s="14"/>
+      <c r="U48" s="14"/>
+      <c r="V48" s="15"/>
+      <c r="W48" s="3"/>
+    </row>
+    <row r="49" spans="1:23" s="4" customFormat="1" ht="12.75">
+      <c r="A49" s="13"/>
+      <c r="B49" s="14"/>
+      <c r="C49" s="14"/>
+      <c r="D49" s="14"/>
+      <c r="E49" s="14"/>
+      <c r="F49" s="14"/>
+      <c r="G49" s="14"/>
+      <c r="H49" s="14"/>
+      <c r="I49" s="14"/>
+      <c r="J49" s="14"/>
+      <c r="K49" s="15"/>
+      <c r="L49" s="13"/>
+      <c r="M49" s="14"/>
+      <c r="N49" s="14"/>
+      <c r="O49" s="14"/>
+      <c r="P49" s="14"/>
+      <c r="Q49" s="14"/>
+      <c r="R49" s="14"/>
+      <c r="S49" s="14"/>
+      <c r="T49" s="14"/>
+      <c r="U49" s="14"/>
+      <c r="V49" s="15"/>
+      <c r="W49" s="3"/>
+    </row>
+    <row r="50" spans="1:23" s="4" customFormat="1" ht="12.75">
+      <c r="A50" s="16"/>
+      <c r="B50" s="14"/>
+      <c r="C50" s="14"/>
+      <c r="D50" s="14"/>
+      <c r="E50" s="14"/>
+      <c r="F50" s="17"/>
+      <c r="G50" s="14"/>
+      <c r="H50" s="14"/>
+      <c r="I50" s="14"/>
+      <c r="J50" s="14"/>
+      <c r="K50" s="15"/>
+      <c r="L50" s="16"/>
+      <c r="M50" s="14"/>
+      <c r="N50" s="14"/>
+      <c r="O50" s="14"/>
+      <c r="P50" s="14"/>
+      <c r="Q50" s="20"/>
+      <c r="R50" s="14"/>
+      <c r="S50" s="14"/>
+      <c r="T50" s="14"/>
+      <c r="U50" s="14"/>
+      <c r="V50" s="15"/>
+      <c r="W50" s="3"/>
+    </row>
+    <row r="51" spans="1:23" s="4" customFormat="1" ht="12.75">
+      <c r="A51" s="13"/>
+      <c r="B51" s="14"/>
+      <c r="C51" s="14"/>
+      <c r="D51" s="14"/>
+      <c r="E51" s="14"/>
+      <c r="F51" s="14"/>
+      <c r="G51" s="14"/>
+      <c r="H51" s="14"/>
+      <c r="I51" s="14"/>
+      <c r="J51" s="14"/>
+      <c r="K51" s="15"/>
+      <c r="L51" s="13"/>
+      <c r="M51" s="14"/>
+      <c r="N51" s="14"/>
+      <c r="O51" s="14"/>
+      <c r="P51" s="14"/>
+      <c r="Q51" s="14"/>
+      <c r="R51" s="14"/>
+      <c r="S51" s="14"/>
+      <c r="T51" s="14"/>
+      <c r="U51" s="14"/>
+      <c r="V51" s="15"/>
+      <c r="W51" s="3"/>
+    </row>
+    <row r="52" spans="1:23" s="4" customFormat="1" ht="12.75">
+      <c r="A52" s="13"/>
+      <c r="B52" s="14"/>
+      <c r="C52" s="14"/>
+      <c r="D52" s="14"/>
+      <c r="E52" s="14"/>
+      <c r="F52" s="14"/>
+      <c r="G52" s="14"/>
+      <c r="H52" s="14"/>
+      <c r="I52" s="14"/>
+      <c r="J52" s="14"/>
+      <c r="K52" s="15"/>
+      <c r="L52" s="13"/>
+      <c r="M52" s="14"/>
+      <c r="N52" s="14"/>
+      <c r="O52" s="14"/>
+      <c r="P52" s="14"/>
+      <c r="Q52" s="14"/>
+      <c r="R52" s="14"/>
+      <c r="S52" s="14"/>
+      <c r="T52" s="14"/>
+      <c r="U52" s="14"/>
+      <c r="V52" s="15"/>
+      <c r="W52" s="3"/>
+    </row>
+    <row r="53" spans="1:23" s="4" customFormat="1" ht="12.75">
+      <c r="A53" s="13"/>
+      <c r="B53" s="14"/>
+      <c r="C53" s="14"/>
+      <c r="D53" s="14"/>
+      <c r="E53" s="14"/>
+      <c r="F53" s="14"/>
+      <c r="G53" s="14"/>
+      <c r="H53" s="14"/>
+      <c r="I53" s="14"/>
+      <c r="J53" s="14"/>
+      <c r="K53" s="15"/>
+      <c r="L53" s="13"/>
+      <c r="M53" s="14"/>
+      <c r="N53" s="14"/>
+      <c r="O53" s="14"/>
+      <c r="P53" s="14"/>
+      <c r="Q53" s="14"/>
+      <c r="R53" s="14"/>
+      <c r="S53" s="14"/>
+      <c r="T53" s="14"/>
+      <c r="U53" s="14"/>
+      <c r="V53" s="15"/>
+      <c r="W53" s="3"/>
+    </row>
+    <row r="54" spans="1:23" s="4" customFormat="1" ht="12.75">
+      <c r="A54" s="13"/>
+      <c r="B54" s="14"/>
+      <c r="C54" s="14"/>
+      <c r="D54" s="14"/>
+      <c r="E54" s="14"/>
+      <c r="F54" s="14"/>
+      <c r="G54" s="14"/>
+      <c r="H54" s="14"/>
+      <c r="I54" s="14"/>
+      <c r="J54" s="14"/>
+      <c r="K54" s="15"/>
+      <c r="L54" s="13"/>
+      <c r="M54" s="14"/>
+      <c r="N54" s="14"/>
+      <c r="O54" s="14"/>
+      <c r="P54" s="14"/>
+      <c r="Q54" s="14"/>
+      <c r="R54" s="14"/>
+      <c r="S54" s="14"/>
+      <c r="T54" s="14"/>
+      <c r="U54" s="14"/>
+      <c r="V54" s="15"/>
+      <c r="W54" s="3"/>
+    </row>
+    <row r="55" spans="1:23" s="4" customFormat="1" ht="12.75">
+      <c r="A55" s="13"/>
+      <c r="B55" s="14"/>
+      <c r="C55" s="14"/>
+      <c r="D55" s="14"/>
+      <c r="E55" s="14"/>
+      <c r="F55" s="14"/>
+      <c r="G55" s="14"/>
+      <c r="H55" s="14"/>
+      <c r="I55" s="14"/>
+      <c r="J55" s="14"/>
+      <c r="K55" s="15"/>
+      <c r="L55" s="13"/>
+      <c r="M55" s="14"/>
+      <c r="N55" s="14"/>
+      <c r="O55" s="14"/>
+      <c r="P55" s="14"/>
+      <c r="Q55" s="14"/>
+      <c r="R55" s="14"/>
+      <c r="S55" s="14"/>
+      <c r="T55" s="14"/>
+      <c r="U55" s="14"/>
+      <c r="V55" s="15"/>
+      <c r="W55" s="3"/>
+    </row>
+    <row r="56" spans="1:23" s="4" customFormat="1" ht="12.75">
+      <c r="A56" s="13"/>
+      <c r="B56" s="14"/>
+      <c r="C56" s="14"/>
+      <c r="D56" s="14"/>
+      <c r="E56" s="14"/>
+      <c r="F56" s="14"/>
+      <c r="G56" s="14"/>
+      <c r="H56" s="14"/>
+      <c r="I56" s="14"/>
+      <c r="J56" s="14"/>
+      <c r="K56" s="15"/>
+      <c r="L56" s="13"/>
+      <c r="M56" s="14"/>
+      <c r="N56" s="14"/>
+      <c r="O56" s="14"/>
+      <c r="P56" s="14"/>
+      <c r="Q56" s="14"/>
+      <c r="R56" s="14"/>
+      <c r="S56" s="14"/>
+      <c r="T56" s="14"/>
+      <c r="U56" s="14"/>
+      <c r="V56" s="15"/>
+      <c r="W56" s="3"/>
+    </row>
+    <row r="57" spans="1:23" s="4" customFormat="1" ht="12.75">
+      <c r="A57" s="13"/>
+      <c r="B57" s="14"/>
+      <c r="C57" s="14"/>
+      <c r="D57" s="14"/>
+      <c r="E57" s="14"/>
+      <c r="F57" s="14"/>
+      <c r="G57" s="14"/>
+      <c r="H57" s="14"/>
+      <c r="I57" s="14"/>
+      <c r="J57" s="14"/>
+      <c r="K57" s="15"/>
+      <c r="L57" s="13"/>
+      <c r="M57" s="14"/>
+      <c r="N57" s="14"/>
+      <c r="O57" s="14"/>
+      <c r="P57" s="14"/>
+      <c r="Q57" s="14"/>
+      <c r="R57" s="14"/>
+      <c r="S57" s="14"/>
+      <c r="T57" s="14"/>
+      <c r="U57" s="14"/>
+      <c r="V57" s="15"/>
+      <c r="W57" s="3"/>
+    </row>
+    <row r="58" spans="1:23" s="4" customFormat="1" ht="12.75">
+      <c r="A58" s="13"/>
+      <c r="B58" s="14"/>
+      <c r="C58" s="14"/>
+      <c r="D58" s="14"/>
+      <c r="E58" s="14"/>
+      <c r="F58" s="14"/>
+      <c r="G58" s="14"/>
+      <c r="H58" s="14"/>
+      <c r="I58" s="14"/>
+      <c r="J58" s="14"/>
+      <c r="K58" s="15"/>
+      <c r="L58" s="13"/>
+      <c r="M58" s="14"/>
+      <c r="N58" s="14"/>
+      <c r="O58" s="14"/>
+      <c r="P58" s="14"/>
+      <c r="Q58" s="14"/>
+      <c r="R58" s="14"/>
+      <c r="S58" s="14"/>
+      <c r="T58" s="14"/>
+      <c r="U58" s="14"/>
+      <c r="V58" s="15"/>
+      <c r="W58" s="3"/>
+    </row>
+    <row r="59" spans="1:23" s="4" customFormat="1" ht="12.75">
+      <c r="A59" s="13"/>
+      <c r="B59" s="14"/>
+      <c r="C59" s="14"/>
+      <c r="D59" s="14"/>
+      <c r="E59" s="14"/>
+      <c r="F59" s="14"/>
+      <c r="G59" s="14"/>
+      <c r="H59" s="14"/>
+      <c r="I59" s="14"/>
+      <c r="J59" s="14"/>
+      <c r="K59" s="15"/>
+      <c r="L59" s="13"/>
+      <c r="M59" s="14"/>
+      <c r="N59" s="14"/>
+      <c r="O59" s="14"/>
+      <c r="P59" s="14"/>
+      <c r="Q59" s="14"/>
+      <c r="R59" s="14"/>
+      <c r="S59" s="14"/>
+      <c r="T59" s="14"/>
+      <c r="U59" s="14"/>
+      <c r="V59" s="15"/>
+      <c r="W59" s="3"/>
+    </row>
+    <row r="60" spans="1:23" s="4" customFormat="1" ht="12.75">
+      <c r="A60" s="13"/>
+      <c r="B60" s="14"/>
+      <c r="C60" s="14"/>
+      <c r="D60" s="14"/>
+      <c r="E60" s="14"/>
+      <c r="F60" s="14"/>
+      <c r="G60" s="14"/>
+      <c r="H60" s="14"/>
+      <c r="I60" s="14"/>
+      <c r="J60" s="14"/>
+      <c r="K60" s="15"/>
+      <c r="L60" s="13"/>
+      <c r="M60" s="14"/>
+      <c r="N60" s="14"/>
+      <c r="O60" s="14"/>
+      <c r="P60" s="14"/>
+      <c r="Q60" s="14"/>
+      <c r="R60" s="14"/>
+      <c r="S60" s="14"/>
+      <c r="T60" s="14"/>
+      <c r="U60" s="14"/>
+      <c r="V60" s="15"/>
+      <c r="W60" s="3"/>
+    </row>
+    <row r="61" spans="1:23" s="4" customFormat="1" ht="12.75">
+      <c r="A61" s="13"/>
+      <c r="B61" s="14"/>
+      <c r="C61" s="14"/>
+      <c r="D61" s="14"/>
+      <c r="E61" s="14"/>
+      <c r="F61" s="14"/>
+      <c r="G61" s="14"/>
+      <c r="H61" s="14"/>
+      <c r="I61" s="14"/>
+      <c r="J61" s="14"/>
+      <c r="K61" s="15"/>
+      <c r="L61" s="13"/>
+      <c r="M61" s="14"/>
+      <c r="N61" s="14"/>
+      <c r="O61" s="14"/>
+      <c r="P61" s="14"/>
+      <c r="Q61" s="14"/>
+      <c r="R61" s="14"/>
+      <c r="S61" s="14"/>
+      <c r="T61" s="14"/>
+      <c r="U61" s="14"/>
+      <c r="V61" s="15"/>
+      <c r="W61" s="3"/>
+    </row>
+    <row r="62" spans="1:23" s="4" customFormat="1" ht="12.75">
+      <c r="A62" s="13"/>
+      <c r="B62" s="14"/>
+      <c r="C62" s="14"/>
+      <c r="D62" s="14"/>
+      <c r="E62" s="14"/>
+      <c r="F62" s="14"/>
+      <c r="G62" s="14"/>
+      <c r="H62" s="14"/>
+      <c r="I62" s="14"/>
+      <c r="J62" s="14"/>
+      <c r="K62" s="15"/>
+      <c r="L62" s="13"/>
+      <c r="M62" s="14"/>
+      <c r="N62" s="14"/>
+      <c r="O62" s="14"/>
+      <c r="P62" s="14"/>
+      <c r="Q62" s="14"/>
+      <c r="R62" s="14"/>
+      <c r="S62" s="14"/>
+      <c r="T62" s="14"/>
+      <c r="U62" s="14"/>
+      <c r="V62" s="15"/>
+      <c r="W62" s="3"/>
+    </row>
+    <row r="63" spans="1:23" s="4" customFormat="1" ht="12.75">
+      <c r="A63" s="13"/>
+      <c r="B63" s="14"/>
+      <c r="C63" s="14"/>
+      <c r="D63" s="14"/>
+      <c r="E63" s="14"/>
+      <c r="F63" s="14"/>
+      <c r="G63" s="14"/>
+      <c r="H63" s="14"/>
+      <c r="I63" s="14"/>
+      <c r="J63" s="14"/>
+      <c r="K63" s="15"/>
+      <c r="L63" s="13"/>
+      <c r="M63" s="14"/>
+      <c r="N63" s="14"/>
+      <c r="O63" s="14"/>
+      <c r="P63" s="14"/>
+      <c r="Q63" s="14"/>
+      <c r="R63" s="14"/>
+      <c r="S63" s="14"/>
+      <c r="T63" s="14"/>
+      <c r="U63" s="14"/>
+      <c r="V63" s="15"/>
+      <c r="W63" s="3"/>
+    </row>
+    <row r="64" spans="1:23" s="4" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A64" s="13"/>
+      <c r="B64" s="14"/>
+      <c r="C64" s="14"/>
+      <c r="D64" s="14"/>
+      <c r="E64" s="14"/>
+      <c r="F64" s="14"/>
+      <c r="G64" s="14"/>
+      <c r="H64" s="14"/>
+      <c r="I64" s="14"/>
+      <c r="J64" s="14"/>
+      <c r="K64" s="15"/>
+      <c r="L64" s="13"/>
+      <c r="M64" s="14"/>
+      <c r="N64" s="14"/>
+      <c r="O64" s="14"/>
+      <c r="P64" s="14"/>
+      <c r="Q64" s="14"/>
+      <c r="R64" s="14"/>
+      <c r="S64" s="14"/>
+      <c r="T64" s="14"/>
+      <c r="U64" s="14"/>
+      <c r="V64" s="15"/>
+      <c r="W64" s="3"/>
+    </row>
+    <row r="65" spans="1:23" s="4" customFormat="1" ht="12.75">
+      <c r="A65" s="13"/>
+      <c r="B65" s="14"/>
+      <c r="C65" s="14"/>
+      <c r="D65" s="14"/>
+      <c r="E65" s="14"/>
+      <c r="F65" s="14"/>
+      <c r="G65" s="14"/>
+      <c r="H65" s="14"/>
+      <c r="I65" s="14"/>
+      <c r="J65" s="14"/>
+      <c r="K65" s="15"/>
+      <c r="L65" s="13"/>
+      <c r="M65" s="14"/>
+      <c r="N65" s="14"/>
+      <c r="O65" s="14"/>
+      <c r="P65" s="14"/>
+      <c r="Q65" s="14"/>
+      <c r="R65" s="14"/>
+      <c r="S65" s="14"/>
+      <c r="T65" s="14"/>
+      <c r="U65" s="14"/>
+      <c r="V65" s="15"/>
+      <c r="W65" s="3"/>
+    </row>
+    <row r="66" spans="1:23" s="4" customFormat="1" ht="12.75">
+      <c r="A66" s="13"/>
+      <c r="B66" s="14"/>
+      <c r="C66" s="14"/>
+      <c r="D66" s="14"/>
+      <c r="E66" s="14"/>
+      <c r="F66" s="14"/>
+      <c r="G66" s="14"/>
+      <c r="H66" s="14"/>
+      <c r="I66" s="14"/>
+      <c r="J66" s="14"/>
+      <c r="K66" s="15"/>
+      <c r="L66" s="13"/>
+      <c r="M66" s="14"/>
+      <c r="N66" s="14"/>
+      <c r="O66" s="14"/>
+      <c r="P66" s="14"/>
+      <c r="Q66" s="14"/>
+      <c r="R66" s="14"/>
+      <c r="S66" s="14"/>
+      <c r="T66" s="14"/>
+      <c r="U66" s="14"/>
+      <c r="V66" s="15"/>
+      <c r="W66" s="3"/>
+    </row>
+    <row r="67" spans="1:23" s="4" customFormat="1" ht="12.75">
+      <c r="A67" s="16"/>
+      <c r="B67" s="14"/>
+      <c r="C67" s="14"/>
+      <c r="D67" s="20"/>
+      <c r="E67" s="14"/>
+      <c r="F67" s="14"/>
+      <c r="G67" s="14"/>
+      <c r="H67" s="17"/>
+      <c r="I67" s="14"/>
+      <c r="J67" s="14"/>
+      <c r="K67" s="15"/>
+      <c r="L67" s="16"/>
+      <c r="M67" s="14"/>
+      <c r="N67" s="14"/>
+      <c r="O67" s="20"/>
+      <c r="P67" s="14"/>
+      <c r="Q67" s="14"/>
+      <c r="R67" s="14"/>
+      <c r="S67" s="17"/>
+      <c r="T67" s="14"/>
+      <c r="U67" s="14"/>
+      <c r="V67" s="15"/>
+      <c r="W67" s="3"/>
+    </row>
+    <row r="68" spans="1:23" s="4" customFormat="1" ht="12.75">
+      <c r="A68" s="13"/>
+      <c r="B68" s="14"/>
+      <c r="C68" s="14"/>
+      <c r="D68" s="14"/>
+      <c r="E68" s="14"/>
+      <c r="F68" s="14"/>
+      <c r="G68" s="14"/>
+      <c r="H68" s="14"/>
+      <c r="I68" s="14"/>
+      <c r="J68" s="14"/>
+      <c r="K68" s="15"/>
+      <c r="L68" s="13"/>
+      <c r="M68" s="14"/>
+      <c r="N68" s="14"/>
+      <c r="O68" s="14"/>
+      <c r="P68" s="14"/>
+      <c r="Q68" s="14"/>
+      <c r="R68" s="14"/>
+      <c r="S68" s="14"/>
+      <c r="T68" s="14"/>
+      <c r="U68" s="14"/>
+      <c r="V68" s="15"/>
+      <c r="W68" s="3"/>
+    </row>
+    <row r="69" spans="1:23" s="4" customFormat="1" ht="12.75">
+      <c r="A69" s="13"/>
+      <c r="B69" s="14"/>
+      <c r="C69" s="14"/>
+      <c r="D69" s="14"/>
+      <c r="E69" s="14"/>
+      <c r="F69" s="14"/>
+      <c r="G69" s="14"/>
+      <c r="H69" s="14"/>
+      <c r="I69" s="14"/>
+      <c r="J69" s="14"/>
+      <c r="K69" s="15"/>
+      <c r="L69" s="13"/>
+      <c r="M69" s="14"/>
+      <c r="N69" s="14"/>
+      <c r="O69" s="14"/>
+      <c r="P69" s="14"/>
+      <c r="Q69" s="14"/>
+      <c r="R69" s="14"/>
+      <c r="S69" s="14"/>
+      <c r="T69" s="14"/>
+      <c r="U69" s="14"/>
+      <c r="V69" s="15"/>
+      <c r="W69" s="3"/>
+    </row>
+    <row r="70" spans="1:23" s="4" customFormat="1" ht="12.75">
+      <c r="A70" s="13"/>
+      <c r="B70" s="14"/>
+      <c r="C70" s="14"/>
+      <c r="D70" s="14"/>
+      <c r="E70" s="14"/>
+      <c r="F70" s="14"/>
+      <c r="G70" s="14"/>
+      <c r="H70" s="14"/>
+      <c r="I70" s="14"/>
+      <c r="J70" s="14"/>
+      <c r="K70" s="15"/>
+      <c r="L70" s="13"/>
+      <c r="M70" s="14"/>
+      <c r="N70" s="14"/>
+      <c r="O70" s="14"/>
+      <c r="P70" s="14"/>
+      <c r="Q70" s="14"/>
+      <c r="R70" s="14"/>
+      <c r="S70" s="14"/>
+      <c r="T70" s="14"/>
+      <c r="U70" s="14"/>
+      <c r="V70" s="15"/>
+      <c r="W70" s="3"/>
+    </row>
+    <row r="71" spans="1:23" s="4" customFormat="1" ht="12.75">
+      <c r="A71" s="13"/>
+      <c r="B71" s="14"/>
+      <c r="C71" s="14"/>
+      <c r="D71" s="14"/>
+      <c r="E71" s="14"/>
+      <c r="F71" s="14"/>
+      <c r="G71" s="14"/>
+      <c r="H71" s="14"/>
+      <c r="I71" s="14"/>
+      <c r="J71" s="14"/>
+      <c r="K71" s="15"/>
+      <c r="L71" s="13"/>
+      <c r="M71" s="14"/>
+      <c r="N71" s="14"/>
+      <c r="O71" s="14"/>
+      <c r="P71" s="14"/>
+      <c r="Q71" s="14"/>
+      <c r="R71" s="14"/>
+      <c r="S71" s="14"/>
+      <c r="T71" s="14"/>
+      <c r="U71" s="14"/>
+      <c r="V71" s="15"/>
+      <c r="W71" s="3"/>
+    </row>
+    <row r="72" spans="1:23" s="4" customFormat="1" ht="12.75">
+      <c r="A72" s="13"/>
+      <c r="B72" s="14"/>
+      <c r="C72" s="14"/>
+      <c r="D72" s="14"/>
+      <c r="E72" s="14"/>
+      <c r="F72" s="14"/>
+      <c r="G72" s="14"/>
+      <c r="H72" s="14"/>
+      <c r="I72" s="14"/>
+      <c r="J72" s="14"/>
+      <c r="K72" s="15"/>
+      <c r="L72" s="13"/>
+      <c r="M72" s="14"/>
+      <c r="N72" s="14"/>
+      <c r="O72" s="14"/>
+      <c r="P72" s="14"/>
+      <c r="Q72" s="14"/>
+      <c r="R72" s="14"/>
+      <c r="S72" s="14"/>
+      <c r="T72" s="14"/>
+      <c r="U72" s="14"/>
+      <c r="V72" s="15"/>
+      <c r="W72" s="3"/>
+    </row>
+    <row r="73" spans="1:23" s="4" customFormat="1" ht="12.75">
+      <c r="A73" s="13"/>
+      <c r="B73" s="14"/>
+      <c r="C73" s="14"/>
+      <c r="D73" s="14"/>
+      <c r="E73" s="14"/>
+      <c r="F73" s="14"/>
+      <c r="G73" s="14"/>
+      <c r="H73" s="14"/>
+      <c r="I73" s="14"/>
+      <c r="J73" s="14"/>
+      <c r="K73" s="15"/>
+      <c r="L73" s="13"/>
+      <c r="M73" s="14"/>
+      <c r="N73" s="14"/>
+      <c r="O73" s="14"/>
+      <c r="P73" s="14"/>
+      <c r="Q73" s="14"/>
+      <c r="R73" s="14"/>
+      <c r="S73" s="14"/>
+      <c r="T73" s="14"/>
+      <c r="U73" s="14"/>
+      <c r="V73" s="15"/>
+      <c r="W73" s="3"/>
+    </row>
+    <row r="74" spans="1:23" s="4" customFormat="1" ht="12.75">
+      <c r="A74" s="13"/>
+      <c r="B74" s="14"/>
+      <c r="C74" s="14"/>
+      <c r="D74" s="14"/>
+      <c r="E74" s="14"/>
+      <c r="F74" s="14"/>
+      <c r="G74" s="14"/>
+      <c r="H74" s="14"/>
+      <c r="I74" s="14"/>
+      <c r="J74" s="14"/>
+      <c r="K74" s="15"/>
+      <c r="L74" s="13"/>
+      <c r="M74" s="14"/>
+      <c r="N74" s="14"/>
+      <c r="O74" s="14"/>
+      <c r="P74" s="14"/>
+      <c r="Q74" s="14"/>
+      <c r="R74" s="14"/>
+      <c r="S74" s="14"/>
+      <c r="T74" s="14"/>
+      <c r="U74" s="14"/>
+      <c r="V74" s="15"/>
+      <c r="W74" s="3"/>
+    </row>
+    <row r="75" spans="1:23" s="4" customFormat="1" ht="12.75">
+      <c r="A75" s="13"/>
+      <c r="B75" s="14"/>
+      <c r="C75" s="14"/>
+      <c r="D75" s="14"/>
+      <c r="E75" s="14"/>
+      <c r="F75" s="14"/>
+      <c r="G75" s="14"/>
+      <c r="H75" s="14"/>
+      <c r="I75" s="14"/>
+      <c r="J75" s="14"/>
+      <c r="K75" s="15"/>
+      <c r="L75" s="13"/>
+      <c r="M75" s="14"/>
+      <c r="N75" s="14"/>
+      <c r="O75" s="14"/>
+      <c r="P75" s="14"/>
+      <c r="Q75" s="14"/>
+      <c r="R75" s="14"/>
+      <c r="S75" s="14"/>
+      <c r="T75" s="14"/>
+      <c r="U75" s="14"/>
+      <c r="V75" s="15"/>
+      <c r="W75" s="3"/>
+    </row>
+    <row r="76" spans="1:23" s="4" customFormat="1" ht="12.75">
+      <c r="A76" s="13"/>
+      <c r="B76" s="14"/>
+      <c r="C76" s="14"/>
+      <c r="D76" s="14"/>
+      <c r="E76" s="14"/>
+      <c r="F76" s="14"/>
+      <c r="G76" s="14"/>
+      <c r="H76" s="14"/>
+      <c r="I76" s="14"/>
+      <c r="J76" s="14"/>
+      <c r="K76" s="15"/>
+      <c r="L76" s="13"/>
+      <c r="M76" s="14"/>
+      <c r="N76" s="14"/>
+      <c r="O76" s="14"/>
+      <c r="P76" s="14"/>
+      <c r="Q76" s="14"/>
+      <c r="R76" s="14"/>
+      <c r="S76" s="14"/>
+      <c r="T76" s="14"/>
+      <c r="U76" s="14"/>
+      <c r="V76" s="15"/>
+      <c r="W76" s="3"/>
+    </row>
+    <row r="77" spans="1:23" s="4" customFormat="1" ht="12.75">
+      <c r="A77" s="13"/>
+      <c r="B77" s="14"/>
+      <c r="C77" s="14"/>
+      <c r="D77" s="14"/>
+      <c r="E77" s="14"/>
+      <c r="F77" s="14"/>
+      <c r="G77" s="14"/>
+      <c r="H77" s="14"/>
+      <c r="I77" s="14"/>
+      <c r="J77" s="14"/>
+      <c r="K77" s="15"/>
+      <c r="L77" s="13"/>
+      <c r="M77" s="14"/>
+      <c r="N77" s="14"/>
+      <c r="O77" s="14"/>
+      <c r="P77" s="14"/>
+      <c r="Q77" s="14"/>
+      <c r="R77" s="14"/>
+      <c r="S77" s="14"/>
+      <c r="T77" s="14"/>
+      <c r="U77" s="14"/>
+      <c r="V77" s="15"/>
+      <c r="W77" s="3"/>
+    </row>
+    <row r="78" spans="1:23" s="4" customFormat="1" ht="12.75">
+      <c r="A78" s="22"/>
+      <c r="B78" s="18"/>
+      <c r="C78" s="18"/>
+      <c r="D78" s="18"/>
+      <c r="E78" s="18"/>
+      <c r="F78" s="18"/>
+      <c r="G78" s="18"/>
+      <c r="H78" s="18"/>
+      <c r="I78" s="18"/>
+      <c r="J78" s="18"/>
+      <c r="K78" s="19"/>
+      <c r="L78" s="22"/>
+      <c r="M78" s="18"/>
+      <c r="N78" s="18"/>
+      <c r="O78" s="18"/>
+      <c r="P78" s="18"/>
+      <c r="Q78" s="18"/>
+      <c r="R78" s="18"/>
+      <c r="S78" s="18"/>
+      <c r="T78" s="18"/>
+      <c r="U78" s="18"/>
+      <c r="V78" s="19"/>
+      <c r="W78" s="3"/>
+    </row>
+    <row r="79" spans="1:23">
+      <c r="A79" s="38" t="s">
+        <v>1</v>
+      </c>
+      <c r="B79" s="39"/>
+      <c r="C79" s="39"/>
+      <c r="D79" s="39"/>
+      <c r="E79" s="39"/>
+      <c r="F79" s="39"/>
+      <c r="G79" s="39"/>
+      <c r="H79" s="39"/>
+      <c r="I79" s="39"/>
+      <c r="J79" s="39"/>
+      <c r="K79" s="40"/>
+      <c r="L79" s="38" t="s">
+        <v>1</v>
+      </c>
+      <c r="M79" s="39"/>
+      <c r="N79" s="39"/>
+      <c r="O79" s="39"/>
+      <c r="P79" s="39"/>
+      <c r="Q79" s="39"/>
+      <c r="R79" s="39"/>
+      <c r="S79" s="39"/>
+      <c r="T79" s="39"/>
+      <c r="U79" s="39"/>
+      <c r="V79" s="40"/>
+    </row>
+    <row r="80" spans="1:23">
+      <c r="A80" s="24"/>
+      <c r="B80" s="5"/>
+      <c r="C80" s="5"/>
+      <c r="D80" s="5"/>
+      <c r="E80" s="5"/>
+      <c r="F80" s="5"/>
+      <c r="G80" s="5"/>
+      <c r="H80" s="5"/>
+      <c r="I80" s="5"/>
+      <c r="J80" s="5"/>
+      <c r="K80" s="6"/>
+      <c r="L80" s="24"/>
+      <c r="M80" s="5"/>
+      <c r="N80" s="5"/>
+      <c r="O80" s="5"/>
+      <c r="P80" s="5"/>
+      <c r="Q80" s="5"/>
+      <c r="R80" s="5"/>
+      <c r="S80" s="5"/>
+      <c r="T80" s="5"/>
+      <c r="U80" s="5"/>
+      <c r="V80" s="6"/>
+    </row>
+    <row r="81" spans="1:22">
+      <c r="A81" s="16"/>
+      <c r="B81" s="7"/>
+      <c r="C81" s="7"/>
+      <c r="D81" s="7"/>
+      <c r="E81" s="7"/>
+      <c r="F81" s="7"/>
+      <c r="G81" s="7"/>
+      <c r="H81" s="7"/>
+      <c r="I81" s="7"/>
+      <c r="J81" s="7"/>
+      <c r="K81" s="8"/>
+      <c r="L81" s="16"/>
+      <c r="M81" s="7"/>
+      <c r="N81" s="7"/>
+      <c r="O81" s="7"/>
+      <c r="P81" s="7"/>
+      <c r="Q81" s="7"/>
+      <c r="R81" s="7"/>
+      <c r="S81" s="7"/>
+      <c r="T81" s="7"/>
+      <c r="U81" s="7"/>
+      <c r="V81" s="8"/>
+    </row>
+    <row r="82" spans="1:22">
+      <c r="A82" s="16"/>
+      <c r="B82" s="7"/>
+      <c r="C82" s="7"/>
+      <c r="D82" s="7"/>
+      <c r="E82" s="7"/>
+      <c r="F82" s="7"/>
+      <c r="G82" s="7"/>
+      <c r="H82" s="7"/>
+      <c r="I82" s="7"/>
+      <c r="J82" s="7"/>
+      <c r="K82" s="8"/>
+      <c r="L82" s="16"/>
+      <c r="M82" s="7"/>
+      <c r="N82" s="7"/>
+      <c r="O82" s="7"/>
+      <c r="P82" s="7"/>
+      <c r="Q82" s="7"/>
+      <c r="R82" s="7"/>
+      <c r="S82" s="7"/>
+      <c r="T82" s="7"/>
+      <c r="U82" s="7"/>
+      <c r="V82" s="8"/>
+    </row>
+    <row r="83" spans="1:22">
+      <c r="A83" s="25"/>
+      <c r="B83" s="9"/>
+      <c r="C83" s="9"/>
+      <c r="D83" s="9"/>
+      <c r="E83" s="9"/>
+      <c r="F83" s="9"/>
+      <c r="G83" s="9"/>
+      <c r="H83" s="9"/>
+      <c r="I83" s="9"/>
+      <c r="J83" s="9"/>
+      <c r="K83" s="10"/>
+      <c r="L83" s="25"/>
+      <c r="M83" s="9"/>
+      <c r="N83" s="9"/>
+      <c r="O83" s="9"/>
+      <c r="P83" s="9"/>
+      <c r="Q83" s="9"/>
+      <c r="R83" s="9"/>
+      <c r="S83" s="9"/>
+      <c r="T83" s="9"/>
+      <c r="U83" s="9"/>
+      <c r="V83" s="10"/>
+    </row>
+  </sheetData>
+  <mergeCells count="51">
+    <mergeCell ref="F31:H31"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E19:H19"/>
+    <mergeCell ref="D20:I20"/>
+    <mergeCell ref="D21:I21"/>
+    <mergeCell ref="D22:I22"/>
+    <mergeCell ref="D23:I23"/>
+    <mergeCell ref="D24:I24"/>
+    <mergeCell ref="D25:I25"/>
+    <mergeCell ref="D26:I26"/>
+    <mergeCell ref="D27:I27"/>
+    <mergeCell ref="D28:I28"/>
+    <mergeCell ref="D29:I29"/>
+    <mergeCell ref="A13:K13"/>
+    <mergeCell ref="A15:K15"/>
+    <mergeCell ref="A16:K16"/>
+    <mergeCell ref="A42:K42"/>
+    <mergeCell ref="L42:V42"/>
+    <mergeCell ref="A79:K79"/>
+    <mergeCell ref="L79:V79"/>
+    <mergeCell ref="A14:K14"/>
+    <mergeCell ref="L14:V14"/>
+    <mergeCell ref="A17:K17"/>
+    <mergeCell ref="L17:V17"/>
+    <mergeCell ref="A37:K37"/>
+    <mergeCell ref="L37:V37"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="D9:H9"/>
+    <mergeCell ref="I9:K9"/>
+    <mergeCell ref="A10:C11"/>
+    <mergeCell ref="D10:H10"/>
+    <mergeCell ref="I10:K10"/>
+    <mergeCell ref="D11:H11"/>
+    <mergeCell ref="I11:K11"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="I6:K6"/>
+    <mergeCell ref="A7:C8"/>
+    <mergeCell ref="I7:K7"/>
+    <mergeCell ref="D8:H8"/>
+    <mergeCell ref="I8:K8"/>
+    <mergeCell ref="D6:H6"/>
+    <mergeCell ref="D7:H7"/>
+    <mergeCell ref="A1:K2"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="I4:K4"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="D5:H5"/>
+    <mergeCell ref="I5:K5"/>
+  </mergeCells>
+  <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:W98"/>
+  <sheetViews>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="18"/>
+  <cols>
+    <col min="1" max="22" width="9.140625" style="2" customWidth="1"/>
+    <col min="23" max="23" width="12.7109375" style="2" customWidth="1"/>
+    <col min="24" max="16384" width="9.140625" style="1" hidden="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:23">
+      <c r="A1" s="55" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="56"/>
+      <c r="H1" s="56"/>
+      <c r="I1" s="56"/>
+      <c r="J1" s="56"/>
+      <c r="K1" s="57"/>
+      <c r="L1" s="29"/>
+      <c r="M1" s="29"/>
+      <c r="N1" s="29"/>
+      <c r="O1" s="29"/>
+      <c r="P1" s="29"/>
+      <c r="Q1" s="29"/>
+      <c r="R1" s="29"/>
+      <c r="S1" s="29"/>
+      <c r="T1" s="29"/>
+      <c r="U1" s="29"/>
+      <c r="V1" s="29"/>
+    </row>
+    <row r="2" spans="1:23">
+      <c r="A2" s="58"/>
+      <c r="B2" s="59"/>
+      <c r="C2" s="59"/>
+      <c r="D2" s="59"/>
+      <c r="E2" s="59"/>
+      <c r="F2" s="59"/>
+      <c r="G2" s="59"/>
+      <c r="H2" s="59"/>
+      <c r="I2" s="59"/>
+      <c r="J2" s="59"/>
+      <c r="K2" s="60"/>
+      <c r="L2" s="29"/>
+      <c r="M2" s="29"/>
+      <c r="N2" s="29"/>
+      <c r="O2" s="29"/>
+      <c r="P2" s="29"/>
+      <c r="Q2" s="29"/>
+      <c r="R2" s="29"/>
+      <c r="S2" s="29"/>
+      <c r="T2" s="29"/>
+      <c r="U2" s="29"/>
+      <c r="V2" s="29"/>
+    </row>
+    <row r="3" spans="1:23">
+      <c r="A3" s="64"/>
+      <c r="B3" s="64"/>
+      <c r="C3" s="64"/>
+      <c r="D3" s="64"/>
+      <c r="E3" s="64"/>
+      <c r="F3" s="64"/>
+      <c r="G3" s="64"/>
+      <c r="H3" s="64"/>
+      <c r="I3" s="64"/>
+      <c r="J3" s="64"/>
+      <c r="K3" s="64"/>
+      <c r="L3" s="29"/>
+      <c r="M3" s="29"/>
+      <c r="N3" s="29"/>
+      <c r="O3" s="29"/>
+      <c r="P3" s="29"/>
+      <c r="Q3" s="29"/>
+      <c r="R3" s="29"/>
+      <c r="S3" s="29"/>
+      <c r="T3" s="29"/>
+      <c r="U3" s="29"/>
+      <c r="V3" s="29"/>
+    </row>
+    <row r="4" spans="1:23">
+      <c r="A4" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" s="36"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="35" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="37"/>
+      <c r="F4" s="26">
+        <v>4</v>
+      </c>
+      <c r="G4" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="H4" s="27">
+        <v>40778</v>
+      </c>
+      <c r="I4" s="35" t="s">
+        <v>3</v>
+      </c>
+      <c r="J4" s="36"/>
+      <c r="K4" s="37"/>
+      <c r="L4" s="30"/>
+      <c r="M4" s="30"/>
+      <c r="N4" s="30"/>
+      <c r="O4" s="30"/>
+      <c r="P4" s="30"/>
+      <c r="Q4" s="30"/>
+      <c r="R4" s="30"/>
+      <c r="S4" s="30"/>
+      <c r="T4" s="30"/>
+      <c r="U4" s="30"/>
+      <c r="V4" s="30"/>
+    </row>
+    <row r="5" spans="1:23" ht="18" customHeight="1">
+      <c r="A5" s="65"/>
+      <c r="B5" s="66"/>
+      <c r="C5" s="67"/>
+      <c r="D5" s="35" t="s">
+        <v>37</v>
+      </c>
+      <c r="E5" s="36"/>
+      <c r="F5" s="36"/>
+      <c r="G5" s="36"/>
+      <c r="H5" s="37"/>
+      <c r="I5" s="68"/>
+      <c r="J5" s="69"/>
+      <c r="K5" s="70"/>
       <c r="L5" s="28"/>
       <c r="M5" s="28"/>
       <c r="N5" s="28"/>
@@ -9738,21 +12338,21 @@
       <c r="V5" s="28"/>
     </row>
     <row r="6" spans="1:23" ht="18" customHeight="1">
-      <c r="A6" s="38" t="s">
+      <c r="A6" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="40"/>
-      <c r="C6" s="39"/>
-      <c r="D6" s="54"/>
-      <c r="E6" s="55"/>
-      <c r="F6" s="55"/>
-      <c r="G6" s="55"/>
-      <c r="H6" s="56"/>
-      <c r="I6" s="70" t="s">
+      <c r="B6" s="36"/>
+      <c r="C6" s="37"/>
+      <c r="D6" s="46"/>
+      <c r="E6" s="47"/>
+      <c r="F6" s="47"/>
+      <c r="G6" s="47"/>
+      <c r="H6" s="48"/>
+      <c r="I6" s="43" t="s">
         <v>49</v>
       </c>
-      <c r="J6" s="71"/>
-      <c r="K6" s="72"/>
+      <c r="J6" s="44"/>
+      <c r="K6" s="45"/>
       <c r="L6" s="28"/>
       <c r="M6" s="28"/>
       <c r="N6" s="28"/>
@@ -9766,19 +12366,19 @@
       <c r="V6" s="28"/>
     </row>
     <row r="7" spans="1:23">
-      <c r="A7" s="54"/>
-      <c r="B7" s="55"/>
-      <c r="C7" s="56"/>
-      <c r="D7" s="57"/>
-      <c r="E7" s="58"/>
-      <c r="F7" s="58"/>
-      <c r="G7" s="58"/>
-      <c r="H7" s="59"/>
-      <c r="I7" s="70" t="s">
+      <c r="A7" s="46"/>
+      <c r="B7" s="47"/>
+      <c r="C7" s="48"/>
+      <c r="D7" s="49"/>
+      <c r="E7" s="50"/>
+      <c r="F7" s="50"/>
+      <c r="G7" s="50"/>
+      <c r="H7" s="51"/>
+      <c r="I7" s="43" t="s">
         <v>56</v>
       </c>
-      <c r="J7" s="71"/>
-      <c r="K7" s="72"/>
+      <c r="J7" s="44"/>
+      <c r="K7" s="45"/>
       <c r="L7" s="28"/>
       <c r="M7" s="28"/>
       <c r="N7" s="28"/>
@@ -9792,19 +12392,19 @@
       <c r="V7" s="28"/>
     </row>
     <row r="8" spans="1:23">
-      <c r="A8" s="57"/>
-      <c r="B8" s="58"/>
-      <c r="C8" s="59"/>
-      <c r="D8" s="38" t="s">
+      <c r="A8" s="49"/>
+      <c r="B8" s="50"/>
+      <c r="C8" s="51"/>
+      <c r="D8" s="35" t="s">
         <v>38</v>
       </c>
-      <c r="E8" s="40"/>
-      <c r="F8" s="40"/>
-      <c r="G8" s="40"/>
-      <c r="H8" s="39"/>
-      <c r="I8" s="70"/>
-      <c r="J8" s="71"/>
-      <c r="K8" s="72"/>
+      <c r="E8" s="36"/>
+      <c r="F8" s="36"/>
+      <c r="G8" s="36"/>
+      <c r="H8" s="37"/>
+      <c r="I8" s="43"/>
+      <c r="J8" s="44"/>
+      <c r="K8" s="45"/>
       <c r="L8" s="28"/>
       <c r="M8" s="28"/>
       <c r="N8" s="28"/>
@@ -9818,19 +12418,19 @@
       <c r="V8" s="28"/>
     </row>
     <row r="9" spans="1:23">
-      <c r="A9" s="38" t="s">
+      <c r="A9" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="40"/>
-      <c r="C9" s="39"/>
-      <c r="D9" s="35"/>
-      <c r="E9" s="36"/>
-      <c r="F9" s="36"/>
-      <c r="G9" s="36"/>
-      <c r="H9" s="37"/>
-      <c r="I9" s="70"/>
-      <c r="J9" s="71"/>
-      <c r="K9" s="72"/>
+      <c r="B9" s="36"/>
+      <c r="C9" s="37"/>
+      <c r="D9" s="65"/>
+      <c r="E9" s="66"/>
+      <c r="F9" s="66"/>
+      <c r="G9" s="66"/>
+      <c r="H9" s="67"/>
+      <c r="I9" s="43"/>
+      <c r="J9" s="44"/>
+      <c r="K9" s="45"/>
       <c r="L9" s="28"/>
       <c r="M9" s="28"/>
       <c r="N9" s="28"/>
@@ -9844,19 +12444,19 @@
       <c r="V9" s="28"/>
     </row>
     <row r="10" spans="1:23">
-      <c r="A10" s="54"/>
-      <c r="B10" s="55"/>
-      <c r="C10" s="56"/>
-      <c r="D10" s="38" t="s">
+      <c r="A10" s="46"/>
+      <c r="B10" s="47"/>
+      <c r="C10" s="48"/>
+      <c r="D10" s="35" t="s">
         <v>36</v>
       </c>
-      <c r="E10" s="40"/>
-      <c r="F10" s="40"/>
-      <c r="G10" s="40"/>
-      <c r="H10" s="39"/>
-      <c r="I10" s="70"/>
-      <c r="J10" s="71"/>
-      <c r="K10" s="72"/>
+      <c r="E10" s="36"/>
+      <c r="F10" s="36"/>
+      <c r="G10" s="36"/>
+      <c r="H10" s="37"/>
+      <c r="I10" s="43"/>
+      <c r="J10" s="44"/>
+      <c r="K10" s="45"/>
       <c r="L10" s="28"/>
       <c r="M10" s="28"/>
       <c r="N10" s="28"/>
@@ -9870,17 +12470,17 @@
       <c r="V10" s="28"/>
     </row>
     <row r="11" spans="1:23">
-      <c r="A11" s="57"/>
-      <c r="B11" s="58"/>
-      <c r="C11" s="59"/>
-      <c r="D11" s="60"/>
-      <c r="E11" s="61"/>
-      <c r="F11" s="61"/>
-      <c r="G11" s="61"/>
-      <c r="H11" s="62"/>
-      <c r="I11" s="73"/>
-      <c r="J11" s="74"/>
-      <c r="K11" s="75"/>
+      <c r="A11" s="49"/>
+      <c r="B11" s="50"/>
+      <c r="C11" s="51"/>
+      <c r="D11" s="61"/>
+      <c r="E11" s="62"/>
+      <c r="F11" s="62"/>
+      <c r="G11" s="62"/>
+      <c r="H11" s="63"/>
+      <c r="I11" s="52"/>
+      <c r="J11" s="53"/>
+      <c r="K11" s="54"/>
       <c r="L11" s="28"/>
       <c r="M11" s="28"/>
       <c r="N11" s="28"/>
@@ -9894,56 +12494,56 @@
       <c r="V11" s="28"/>
     </row>
     <row r="12" spans="1:23">
-      <c r="A12" s="53"/>
-      <c r="B12" s="53"/>
-      <c r="C12" s="53"/>
-      <c r="D12" s="53"/>
-      <c r="E12" s="53"/>
-      <c r="F12" s="53"/>
-      <c r="G12" s="53"/>
-      <c r="H12" s="53"/>
-      <c r="I12" s="53"/>
-      <c r="J12" s="53"/>
-      <c r="K12" s="53"/>
-      <c r="L12" s="66"/>
-      <c r="M12" s="66"/>
-      <c r="N12" s="66"/>
-      <c r="O12" s="66"/>
-      <c r="P12" s="66"/>
-      <c r="Q12" s="66"/>
-      <c r="R12" s="66"/>
-      <c r="S12" s="66"/>
-      <c r="T12" s="66"/>
-      <c r="U12" s="66"/>
-      <c r="V12" s="66"/>
+      <c r="A12" s="42"/>
+      <c r="B12" s="42"/>
+      <c r="C12" s="42"/>
+      <c r="D12" s="42"/>
+      <c r="E12" s="42"/>
+      <c r="F12" s="42"/>
+      <c r="G12" s="42"/>
+      <c r="H12" s="42"/>
+      <c r="I12" s="42"/>
+      <c r="J12" s="42"/>
+      <c r="K12" s="42"/>
+      <c r="L12" s="41"/>
+      <c r="M12" s="41"/>
+      <c r="N12" s="41"/>
+      <c r="O12" s="41"/>
+      <c r="P12" s="41"/>
+      <c r="Q12" s="41"/>
+      <c r="R12" s="41"/>
+      <c r="S12" s="41"/>
+      <c r="T12" s="41"/>
+      <c r="U12" s="41"/>
+      <c r="V12" s="41"/>
     </row>
     <row r="13" spans="1:23" ht="18" customHeight="1">
-      <c r="A13" s="38" t="s">
+      <c r="A13" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="B13" s="40"/>
-      <c r="C13" s="40"/>
-      <c r="D13" s="40"/>
-      <c r="E13" s="40"/>
-      <c r="F13" s="40"/>
-      <c r="G13" s="40"/>
-      <c r="H13" s="40"/>
-      <c r="I13" s="40"/>
-      <c r="J13" s="40"/>
-      <c r="K13" s="39"/>
-      <c r="L13" s="38" t="s">
+      <c r="B13" s="36"/>
+      <c r="C13" s="36"/>
+      <c r="D13" s="36"/>
+      <c r="E13" s="36"/>
+      <c r="F13" s="36"/>
+      <c r="G13" s="36"/>
+      <c r="H13" s="36"/>
+      <c r="I13" s="36"/>
+      <c r="J13" s="36"/>
+      <c r="K13" s="37"/>
+      <c r="L13" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="M13" s="40"/>
-      <c r="N13" s="40"/>
-      <c r="O13" s="40"/>
-      <c r="P13" s="40"/>
-      <c r="Q13" s="40"/>
-      <c r="R13" s="40"/>
-      <c r="S13" s="40"/>
-      <c r="T13" s="40"/>
-      <c r="U13" s="40"/>
-      <c r="V13" s="39"/>
+      <c r="M13" s="36"/>
+      <c r="N13" s="36"/>
+      <c r="O13" s="36"/>
+      <c r="P13" s="36"/>
+      <c r="Q13" s="36"/>
+      <c r="R13" s="36"/>
+      <c r="S13" s="36"/>
+      <c r="T13" s="36"/>
+      <c r="U13" s="36"/>
+      <c r="V13" s="37"/>
     </row>
     <row r="14" spans="1:23" s="4" customFormat="1" ht="18" customHeight="1">
       <c r="A14" s="23"/>
@@ -10846,32 +13446,32 @@
       <c r="W49" s="3"/>
     </row>
     <row r="50" spans="1:23">
-      <c r="A50" s="32" t="s">
+      <c r="A50" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B50" s="33"/>
-      <c r="C50" s="33"/>
-      <c r="D50" s="33"/>
-      <c r="E50" s="33"/>
-      <c r="F50" s="33"/>
-      <c r="G50" s="33"/>
-      <c r="H50" s="33"/>
-      <c r="I50" s="33"/>
-      <c r="J50" s="33"/>
-      <c r="K50" s="34"/>
-      <c r="L50" s="32" t="s">
+      <c r="B50" s="39"/>
+      <c r="C50" s="39"/>
+      <c r="D50" s="39"/>
+      <c r="E50" s="39"/>
+      <c r="F50" s="39"/>
+      <c r="G50" s="39"/>
+      <c r="H50" s="39"/>
+      <c r="I50" s="39"/>
+      <c r="J50" s="39"/>
+      <c r="K50" s="40"/>
+      <c r="L50" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="M50" s="33"/>
-      <c r="N50" s="33"/>
-      <c r="O50" s="33"/>
-      <c r="P50" s="33"/>
-      <c r="Q50" s="33"/>
-      <c r="R50" s="33"/>
-      <c r="S50" s="33"/>
-      <c r="T50" s="33"/>
-      <c r="U50" s="33"/>
-      <c r="V50" s="34"/>
+      <c r="M50" s="39"/>
+      <c r="N50" s="39"/>
+      <c r="O50" s="39"/>
+      <c r="P50" s="39"/>
+      <c r="Q50" s="39"/>
+      <c r="R50" s="39"/>
+      <c r="S50" s="39"/>
+      <c r="T50" s="39"/>
+      <c r="U50" s="39"/>
+      <c r="V50" s="40"/>
     </row>
     <row r="51" spans="1:23">
       <c r="A51" s="24"/>
@@ -10970,32 +13570,32 @@
       <c r="V54" s="10"/>
     </row>
     <row r="57" spans="1:23" ht="18" customHeight="1">
-      <c r="A57" s="38" t="s">
+      <c r="A57" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="B57" s="40"/>
-      <c r="C57" s="40"/>
-      <c r="D57" s="40"/>
-      <c r="E57" s="40"/>
-      <c r="F57" s="40"/>
-      <c r="G57" s="40"/>
-      <c r="H57" s="40"/>
-      <c r="I57" s="40"/>
-      <c r="J57" s="40"/>
-      <c r="K57" s="39"/>
-      <c r="L57" s="38" t="s">
+      <c r="B57" s="36"/>
+      <c r="C57" s="36"/>
+      <c r="D57" s="36"/>
+      <c r="E57" s="36"/>
+      <c r="F57" s="36"/>
+      <c r="G57" s="36"/>
+      <c r="H57" s="36"/>
+      <c r="I57" s="36"/>
+      <c r="J57" s="36"/>
+      <c r="K57" s="37"/>
+      <c r="L57" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="M57" s="40"/>
-      <c r="N57" s="40"/>
-      <c r="O57" s="40"/>
-      <c r="P57" s="40"/>
-      <c r="Q57" s="40"/>
-      <c r="R57" s="40"/>
-      <c r="S57" s="40"/>
-      <c r="T57" s="40"/>
-      <c r="U57" s="40"/>
-      <c r="V57" s="39"/>
+      <c r="M57" s="36"/>
+      <c r="N57" s="36"/>
+      <c r="O57" s="36"/>
+      <c r="P57" s="36"/>
+      <c r="Q57" s="36"/>
+      <c r="R57" s="36"/>
+      <c r="S57" s="36"/>
+      <c r="T57" s="36"/>
+      <c r="U57" s="36"/>
+      <c r="V57" s="37"/>
     </row>
     <row r="58" spans="1:23" s="4" customFormat="1" ht="18" customHeight="1">
       <c r="A58" s="23"/>
@@ -11964,32 +14564,32 @@
       <c r="W93" s="3"/>
     </row>
     <row r="94" spans="1:23">
-      <c r="A94" s="32" t="s">
+      <c r="A94" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B94" s="33"/>
-      <c r="C94" s="33"/>
-      <c r="D94" s="33"/>
-      <c r="E94" s="33"/>
-      <c r="F94" s="33"/>
-      <c r="G94" s="33"/>
-      <c r="H94" s="33"/>
-      <c r="I94" s="33"/>
-      <c r="J94" s="33"/>
-      <c r="K94" s="34"/>
-      <c r="L94" s="32" t="s">
+      <c r="B94" s="39"/>
+      <c r="C94" s="39"/>
+      <c r="D94" s="39"/>
+      <c r="E94" s="39"/>
+      <c r="F94" s="39"/>
+      <c r="G94" s="39"/>
+      <c r="H94" s="39"/>
+      <c r="I94" s="39"/>
+      <c r="J94" s="39"/>
+      <c r="K94" s="40"/>
+      <c r="L94" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="M94" s="33"/>
-      <c r="N94" s="33"/>
-      <c r="O94" s="33"/>
-      <c r="P94" s="33"/>
-      <c r="Q94" s="33"/>
-      <c r="R94" s="33"/>
-      <c r="S94" s="33"/>
-      <c r="T94" s="33"/>
-      <c r="U94" s="33"/>
-      <c r="V94" s="34"/>
+      <c r="M94" s="39"/>
+      <c r="N94" s="39"/>
+      <c r="O94" s="39"/>
+      <c r="P94" s="39"/>
+      <c r="Q94" s="39"/>
+      <c r="R94" s="39"/>
+      <c r="S94" s="39"/>
+      <c r="T94" s="39"/>
+      <c r="U94" s="39"/>
+      <c r="V94" s="40"/>
     </row>
     <row r="95" spans="1:23">
       <c r="A95" s="24" t="s">
@@ -12106,21 +14706,6 @@
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <mergeCells count="33">
-    <mergeCell ref="A57:K57"/>
-    <mergeCell ref="L57:V57"/>
-    <mergeCell ref="A94:K94"/>
-    <mergeCell ref="L94:V94"/>
-    <mergeCell ref="A50:K50"/>
-    <mergeCell ref="A13:K13"/>
-    <mergeCell ref="L13:V13"/>
-    <mergeCell ref="L12:V12"/>
-    <mergeCell ref="L50:V50"/>
-    <mergeCell ref="A12:K12"/>
-    <mergeCell ref="I10:K10"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="D6:H7"/>
-    <mergeCell ref="I7:K7"/>
-    <mergeCell ref="A7:C8"/>
     <mergeCell ref="I11:K11"/>
     <mergeCell ref="A1:K2"/>
     <mergeCell ref="A9:C9"/>
@@ -12137,8 +14722,23 @@
     <mergeCell ref="I5:K5"/>
     <mergeCell ref="I6:K6"/>
     <mergeCell ref="A5:C5"/>
+    <mergeCell ref="I10:K10"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="D6:H7"/>
+    <mergeCell ref="I7:K7"/>
+    <mergeCell ref="A7:C8"/>
     <mergeCell ref="I8:K8"/>
     <mergeCell ref="I9:K9"/>
+    <mergeCell ref="A13:K13"/>
+    <mergeCell ref="L13:V13"/>
+    <mergeCell ref="L12:V12"/>
+    <mergeCell ref="L50:V50"/>
+    <mergeCell ref="A12:K12"/>
+    <mergeCell ref="A57:K57"/>
+    <mergeCell ref="L57:V57"/>
+    <mergeCell ref="A94:K94"/>
+    <mergeCell ref="L94:V94"/>
+    <mergeCell ref="A50:K50"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
@@ -12149,23 +14749,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B42" sqref="B42"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
   <sheetData/>
@@ -12178,7 +14768,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D45" sqref="D45"/>
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
@@ -12192,7 +14782,7 @@
   <dimension ref="A1:W98"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I6" sqref="I6:K6"/>
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="18"/>
@@ -12203,19 +14793,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="55" t="s">
         <v>54</v>
       </c>
-      <c r="B1" s="48"/>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
-      <c r="F1" s="48"/>
-      <c r="G1" s="48"/>
-      <c r="H1" s="48"/>
-      <c r="I1" s="48"/>
-      <c r="J1" s="48"/>
-      <c r="K1" s="49"/>
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="56"/>
+      <c r="H1" s="56"/>
+      <c r="I1" s="56"/>
+      <c r="J1" s="56"/>
+      <c r="K1" s="57"/>
       <c r="L1" s="29"/>
       <c r="M1" s="29"/>
       <c r="N1" s="29"/>
@@ -12229,17 +14819,17 @@
       <c r="V1" s="29"/>
     </row>
     <row r="2" spans="1:23">
-      <c r="A2" s="50"/>
-      <c r="B2" s="51"/>
-      <c r="C2" s="51"/>
-      <c r="D2" s="51"/>
-      <c r="E2" s="51"/>
-      <c r="F2" s="51"/>
-      <c r="G2" s="51"/>
-      <c r="H2" s="51"/>
-      <c r="I2" s="51"/>
-      <c r="J2" s="51"/>
-      <c r="K2" s="52"/>
+      <c r="A2" s="58"/>
+      <c r="B2" s="59"/>
+      <c r="C2" s="59"/>
+      <c r="D2" s="59"/>
+      <c r="E2" s="59"/>
+      <c r="F2" s="59"/>
+      <c r="G2" s="59"/>
+      <c r="H2" s="59"/>
+      <c r="I2" s="59"/>
+      <c r="J2" s="59"/>
+      <c r="K2" s="60"/>
       <c r="L2" s="29"/>
       <c r="M2" s="29"/>
       <c r="N2" s="29"/>
@@ -12253,17 +14843,17 @@
       <c r="V2" s="29"/>
     </row>
     <row r="3" spans="1:23">
-      <c r="A3" s="31"/>
-      <c r="B3" s="31"/>
-      <c r="C3" s="31"/>
-      <c r="D3" s="31"/>
-      <c r="E3" s="31"/>
-      <c r="F3" s="31"/>
-      <c r="G3" s="31"/>
-      <c r="H3" s="31"/>
-      <c r="I3" s="31"/>
-      <c r="J3" s="31"/>
-      <c r="K3" s="31"/>
+      <c r="A3" s="64"/>
+      <c r="B3" s="64"/>
+      <c r="C3" s="64"/>
+      <c r="D3" s="64"/>
+      <c r="E3" s="64"/>
+      <c r="F3" s="64"/>
+      <c r="G3" s="64"/>
+      <c r="H3" s="64"/>
+      <c r="I3" s="64"/>
+      <c r="J3" s="64"/>
+      <c r="K3" s="64"/>
       <c r="L3" s="29"/>
       <c r="M3" s="29"/>
       <c r="N3" s="29"/>
@@ -12277,25 +14867,25 @@
       <c r="V3" s="29"/>
     </row>
     <row r="4" spans="1:23">
-      <c r="A4" s="38" t="s">
+      <c r="A4" s="35" t="s">
         <v>55</v>
       </c>
-      <c r="B4" s="40"/>
-      <c r="C4" s="39"/>
-      <c r="D4" s="38" t="s">
+      <c r="B4" s="36"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="39"/>
+      <c r="E4" s="37"/>
       <c r="F4" s="26"/>
       <c r="G4" s="21" t="s">
         <v>0</v>
       </c>
       <c r="H4" s="27"/>
-      <c r="I4" s="38" t="s">
+      <c r="I4" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="J4" s="40"/>
-      <c r="K4" s="39"/>
+      <c r="J4" s="36"/>
+      <c r="K4" s="37"/>
       <c r="L4" s="30"/>
       <c r="M4" s="30"/>
       <c r="N4" s="30"/>
@@ -12309,21 +14899,21 @@
       <c r="V4" s="30"/>
     </row>
     <row r="5" spans="1:23" ht="18" customHeight="1">
-      <c r="A5" s="35"/>
-      <c r="B5" s="36"/>
-      <c r="C5" s="37"/>
-      <c r="D5" s="38" t="s">
+      <c r="A5" s="65"/>
+      <c r="B5" s="66"/>
+      <c r="C5" s="67"/>
+      <c r="D5" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="E5" s="40"/>
-      <c r="F5" s="40"/>
-      <c r="G5" s="40"/>
-      <c r="H5" s="39"/>
-      <c r="I5" s="41" t="s">
+      <c r="E5" s="36"/>
+      <c r="F5" s="36"/>
+      <c r="G5" s="36"/>
+      <c r="H5" s="37"/>
+      <c r="I5" s="77" t="s">
         <v>41</v>
       </c>
-      <c r="J5" s="42"/>
-      <c r="K5" s="43"/>
+      <c r="J5" s="78"/>
+      <c r="K5" s="79"/>
       <c r="L5" s="28"/>
       <c r="M5" s="28"/>
       <c r="N5" s="28"/>
@@ -12337,21 +14927,21 @@
       <c r="V5" s="28"/>
     </row>
     <row r="6" spans="1:23" ht="18" customHeight="1">
-      <c r="A6" s="38" t="s">
+      <c r="A6" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="40"/>
-      <c r="C6" s="39"/>
-      <c r="D6" s="54"/>
-      <c r="E6" s="55"/>
-      <c r="F6" s="55"/>
-      <c r="G6" s="55"/>
-      <c r="H6" s="56"/>
-      <c r="I6" s="44" t="s">
+      <c r="B6" s="36"/>
+      <c r="C6" s="37"/>
+      <c r="D6" s="46"/>
+      <c r="E6" s="47"/>
+      <c r="F6" s="47"/>
+      <c r="G6" s="47"/>
+      <c r="H6" s="48"/>
+      <c r="I6" s="71" t="s">
         <v>49</v>
       </c>
-      <c r="J6" s="45"/>
-      <c r="K6" s="46"/>
+      <c r="J6" s="72"/>
+      <c r="K6" s="73"/>
       <c r="L6" s="28"/>
       <c r="M6" s="28"/>
       <c r="N6" s="28"/>
@@ -12365,19 +14955,19 @@
       <c r="V6" s="28"/>
     </row>
     <row r="7" spans="1:23">
-      <c r="A7" s="54"/>
-      <c r="B7" s="55"/>
-      <c r="C7" s="56"/>
-      <c r="D7" s="57"/>
-      <c r="E7" s="58"/>
-      <c r="F7" s="58"/>
-      <c r="G7" s="58"/>
-      <c r="H7" s="59"/>
-      <c r="I7" s="44" t="s">
+      <c r="A7" s="46"/>
+      <c r="B7" s="47"/>
+      <c r="C7" s="48"/>
+      <c r="D7" s="49"/>
+      <c r="E7" s="50"/>
+      <c r="F7" s="50"/>
+      <c r="G7" s="50"/>
+      <c r="H7" s="51"/>
+      <c r="I7" s="71" t="s">
         <v>39</v>
       </c>
-      <c r="J7" s="45"/>
-      <c r="K7" s="46"/>
+      <c r="J7" s="72"/>
+      <c r="K7" s="73"/>
       <c r="L7" s="28"/>
       <c r="M7" s="28"/>
       <c r="N7" s="28"/>
@@ -12391,21 +14981,21 @@
       <c r="V7" s="28"/>
     </row>
     <row r="8" spans="1:23">
-      <c r="A8" s="57"/>
-      <c r="B8" s="58"/>
-      <c r="C8" s="59"/>
-      <c r="D8" s="38" t="s">
+      <c r="A8" s="49"/>
+      <c r="B8" s="50"/>
+      <c r="C8" s="51"/>
+      <c r="D8" s="35" t="s">
         <v>38</v>
       </c>
-      <c r="E8" s="40"/>
-      <c r="F8" s="40"/>
-      <c r="G8" s="40"/>
-      <c r="H8" s="39"/>
-      <c r="I8" s="44" t="s">
+      <c r="E8" s="36"/>
+      <c r="F8" s="36"/>
+      <c r="G8" s="36"/>
+      <c r="H8" s="37"/>
+      <c r="I8" s="71" t="s">
         <v>40</v>
       </c>
-      <c r="J8" s="45"/>
-      <c r="K8" s="46"/>
+      <c r="J8" s="72"/>
+      <c r="K8" s="73"/>
       <c r="L8" s="28"/>
       <c r="M8" s="28"/>
       <c r="N8" s="28"/>
@@ -12419,21 +15009,21 @@
       <c r="V8" s="28"/>
     </row>
     <row r="9" spans="1:23">
-      <c r="A9" s="38" t="s">
+      <c r="A9" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="40"/>
-      <c r="C9" s="39"/>
-      <c r="D9" s="35"/>
-      <c r="E9" s="36"/>
-      <c r="F9" s="36"/>
-      <c r="G9" s="36"/>
-      <c r="H9" s="37"/>
-      <c r="I9" s="44" t="s">
+      <c r="B9" s="36"/>
+      <c r="C9" s="37"/>
+      <c r="D9" s="65"/>
+      <c r="E9" s="66"/>
+      <c r="F9" s="66"/>
+      <c r="G9" s="66"/>
+      <c r="H9" s="67"/>
+      <c r="I9" s="71" t="s">
         <v>42</v>
       </c>
-      <c r="J9" s="45"/>
-      <c r="K9" s="46"/>
+      <c r="J9" s="72"/>
+      <c r="K9" s="73"/>
       <c r="L9" s="28"/>
       <c r="M9" s="28"/>
       <c r="N9" s="28"/>
@@ -12447,19 +15037,19 @@
       <c r="V9" s="28"/>
     </row>
     <row r="10" spans="1:23">
-      <c r="A10" s="54"/>
-      <c r="B10" s="55"/>
-      <c r="C10" s="56"/>
-      <c r="D10" s="38" t="s">
+      <c r="A10" s="46"/>
+      <c r="B10" s="47"/>
+      <c r="C10" s="48"/>
+      <c r="D10" s="35" t="s">
         <v>36</v>
       </c>
-      <c r="E10" s="40"/>
-      <c r="F10" s="40"/>
-      <c r="G10" s="40"/>
-      <c r="H10" s="39"/>
-      <c r="I10" s="44"/>
-      <c r="J10" s="45"/>
-      <c r="K10" s="46"/>
+      <c r="E10" s="36"/>
+      <c r="F10" s="36"/>
+      <c r="G10" s="36"/>
+      <c r="H10" s="37"/>
+      <c r="I10" s="71"/>
+      <c r="J10" s="72"/>
+      <c r="K10" s="73"/>
       <c r="L10" s="28"/>
       <c r="M10" s="28"/>
       <c r="N10" s="28"/>
@@ -12473,17 +15063,17 @@
       <c r="V10" s="28"/>
     </row>
     <row r="11" spans="1:23">
-      <c r="A11" s="57"/>
-      <c r="B11" s="58"/>
-      <c r="C11" s="59"/>
-      <c r="D11" s="60"/>
-      <c r="E11" s="61"/>
-      <c r="F11" s="61"/>
-      <c r="G11" s="61"/>
-      <c r="H11" s="62"/>
-      <c r="I11" s="63"/>
-      <c r="J11" s="64"/>
-      <c r="K11" s="65"/>
+      <c r="A11" s="49"/>
+      <c r="B11" s="50"/>
+      <c r="C11" s="51"/>
+      <c r="D11" s="61"/>
+      <c r="E11" s="62"/>
+      <c r="F11" s="62"/>
+      <c r="G11" s="62"/>
+      <c r="H11" s="63"/>
+      <c r="I11" s="74"/>
+      <c r="J11" s="75"/>
+      <c r="K11" s="76"/>
       <c r="L11" s="28"/>
       <c r="M11" s="28"/>
       <c r="N11" s="28"/>
@@ -12497,56 +15087,56 @@
       <c r="V11" s="28"/>
     </row>
     <row r="12" spans="1:23">
-      <c r="A12" s="53"/>
-      <c r="B12" s="53"/>
-      <c r="C12" s="53"/>
-      <c r="D12" s="53"/>
-      <c r="E12" s="53"/>
-      <c r="F12" s="53"/>
-      <c r="G12" s="53"/>
-      <c r="H12" s="53"/>
-      <c r="I12" s="53"/>
-      <c r="J12" s="53"/>
-      <c r="K12" s="53"/>
-      <c r="L12" s="66"/>
-      <c r="M12" s="66"/>
-      <c r="N12" s="66"/>
-      <c r="O12" s="66"/>
-      <c r="P12" s="66"/>
-      <c r="Q12" s="66"/>
-      <c r="R12" s="66"/>
-      <c r="S12" s="66"/>
-      <c r="T12" s="66"/>
-      <c r="U12" s="66"/>
-      <c r="V12" s="66"/>
+      <c r="A12" s="42"/>
+      <c r="B12" s="42"/>
+      <c r="C12" s="42"/>
+      <c r="D12" s="42"/>
+      <c r="E12" s="42"/>
+      <c r="F12" s="42"/>
+      <c r="G12" s="42"/>
+      <c r="H12" s="42"/>
+      <c r="I12" s="42"/>
+      <c r="J12" s="42"/>
+      <c r="K12" s="42"/>
+      <c r="L12" s="41"/>
+      <c r="M12" s="41"/>
+      <c r="N12" s="41"/>
+      <c r="O12" s="41"/>
+      <c r="P12" s="41"/>
+      <c r="Q12" s="41"/>
+      <c r="R12" s="41"/>
+      <c r="S12" s="41"/>
+      <c r="T12" s="41"/>
+      <c r="U12" s="41"/>
+      <c r="V12" s="41"/>
     </row>
     <row r="13" spans="1:23" ht="18" customHeight="1">
-      <c r="A13" s="38" t="s">
+      <c r="A13" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="B13" s="40"/>
-      <c r="C13" s="40"/>
-      <c r="D13" s="40"/>
-      <c r="E13" s="40"/>
-      <c r="F13" s="40"/>
-      <c r="G13" s="40"/>
-      <c r="H13" s="40"/>
-      <c r="I13" s="40"/>
-      <c r="J13" s="40"/>
-      <c r="K13" s="39"/>
-      <c r="L13" s="38" t="s">
+      <c r="B13" s="36"/>
+      <c r="C13" s="36"/>
+      <c r="D13" s="36"/>
+      <c r="E13" s="36"/>
+      <c r="F13" s="36"/>
+      <c r="G13" s="36"/>
+      <c r="H13" s="36"/>
+      <c r="I13" s="36"/>
+      <c r="J13" s="36"/>
+      <c r="K13" s="37"/>
+      <c r="L13" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="M13" s="40"/>
-      <c r="N13" s="40"/>
-      <c r="O13" s="40"/>
-      <c r="P13" s="40"/>
-      <c r="Q13" s="40"/>
-      <c r="R13" s="40"/>
-      <c r="S13" s="40"/>
-      <c r="T13" s="40"/>
-      <c r="U13" s="40"/>
-      <c r="V13" s="39"/>
+      <c r="M13" s="36"/>
+      <c r="N13" s="36"/>
+      <c r="O13" s="36"/>
+      <c r="P13" s="36"/>
+      <c r="Q13" s="36"/>
+      <c r="R13" s="36"/>
+      <c r="S13" s="36"/>
+      <c r="T13" s="36"/>
+      <c r="U13" s="36"/>
+      <c r="V13" s="37"/>
     </row>
     <row r="14" spans="1:23" s="4" customFormat="1" ht="18" customHeight="1">
       <c r="A14" s="23"/>
@@ -13449,32 +16039,32 @@
       <c r="W49" s="3"/>
     </row>
     <row r="50" spans="1:23">
-      <c r="A50" s="32" t="s">
+      <c r="A50" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B50" s="33"/>
-      <c r="C50" s="33"/>
-      <c r="D50" s="33"/>
-      <c r="E50" s="33"/>
-      <c r="F50" s="33"/>
-      <c r="G50" s="33"/>
-      <c r="H50" s="33"/>
-      <c r="I50" s="33"/>
-      <c r="J50" s="33"/>
-      <c r="K50" s="34"/>
-      <c r="L50" s="32" t="s">
+      <c r="B50" s="39"/>
+      <c r="C50" s="39"/>
+      <c r="D50" s="39"/>
+      <c r="E50" s="39"/>
+      <c r="F50" s="39"/>
+      <c r="G50" s="39"/>
+      <c r="H50" s="39"/>
+      <c r="I50" s="39"/>
+      <c r="J50" s="39"/>
+      <c r="K50" s="40"/>
+      <c r="L50" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="M50" s="33"/>
-      <c r="N50" s="33"/>
-      <c r="O50" s="33"/>
-      <c r="P50" s="33"/>
-      <c r="Q50" s="33"/>
-      <c r="R50" s="33"/>
-      <c r="S50" s="33"/>
-      <c r="T50" s="33"/>
-      <c r="U50" s="33"/>
-      <c r="V50" s="34"/>
+      <c r="M50" s="39"/>
+      <c r="N50" s="39"/>
+      <c r="O50" s="39"/>
+      <c r="P50" s="39"/>
+      <c r="Q50" s="39"/>
+      <c r="R50" s="39"/>
+      <c r="S50" s="39"/>
+      <c r="T50" s="39"/>
+      <c r="U50" s="39"/>
+      <c r="V50" s="40"/>
     </row>
     <row r="51" spans="1:23">
       <c r="A51" s="24"/>
@@ -13573,32 +16163,32 @@
       <c r="V54" s="10"/>
     </row>
     <row r="57" spans="1:23" ht="18" customHeight="1">
-      <c r="A57" s="38" t="s">
+      <c r="A57" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="B57" s="40"/>
-      <c r="C57" s="40"/>
-      <c r="D57" s="40"/>
-      <c r="E57" s="40"/>
-      <c r="F57" s="40"/>
-      <c r="G57" s="40"/>
-      <c r="H57" s="40"/>
-      <c r="I57" s="40"/>
-      <c r="J57" s="40"/>
-      <c r="K57" s="39"/>
-      <c r="L57" s="38" t="s">
+      <c r="B57" s="36"/>
+      <c r="C57" s="36"/>
+      <c r="D57" s="36"/>
+      <c r="E57" s="36"/>
+      <c r="F57" s="36"/>
+      <c r="G57" s="36"/>
+      <c r="H57" s="36"/>
+      <c r="I57" s="36"/>
+      <c r="J57" s="36"/>
+      <c r="K57" s="37"/>
+      <c r="L57" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="M57" s="40"/>
-      <c r="N57" s="40"/>
-      <c r="O57" s="40"/>
-      <c r="P57" s="40"/>
-      <c r="Q57" s="40"/>
-      <c r="R57" s="40"/>
-      <c r="S57" s="40"/>
-      <c r="T57" s="40"/>
-      <c r="U57" s="40"/>
-      <c r="V57" s="39"/>
+      <c r="M57" s="36"/>
+      <c r="N57" s="36"/>
+      <c r="O57" s="36"/>
+      <c r="P57" s="36"/>
+      <c r="Q57" s="36"/>
+      <c r="R57" s="36"/>
+      <c r="S57" s="36"/>
+      <c r="T57" s="36"/>
+      <c r="U57" s="36"/>
+      <c r="V57" s="37"/>
     </row>
     <row r="58" spans="1:23" s="4" customFormat="1" ht="18" customHeight="1">
       <c r="A58" s="23"/>
@@ -14567,32 +17157,32 @@
       <c r="W93" s="3"/>
     </row>
     <row r="94" spans="1:23">
-      <c r="A94" s="32" t="s">
+      <c r="A94" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B94" s="33"/>
-      <c r="C94" s="33"/>
-      <c r="D94" s="33"/>
-      <c r="E94" s="33"/>
-      <c r="F94" s="33"/>
-      <c r="G94" s="33"/>
-      <c r="H94" s="33"/>
-      <c r="I94" s="33"/>
-      <c r="J94" s="33"/>
-      <c r="K94" s="34"/>
-      <c r="L94" s="32" t="s">
+      <c r="B94" s="39"/>
+      <c r="C94" s="39"/>
+      <c r="D94" s="39"/>
+      <c r="E94" s="39"/>
+      <c r="F94" s="39"/>
+      <c r="G94" s="39"/>
+      <c r="H94" s="39"/>
+      <c r="I94" s="39"/>
+      <c r="J94" s="39"/>
+      <c r="K94" s="40"/>
+      <c r="L94" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="M94" s="33"/>
-      <c r="N94" s="33"/>
-      <c r="O94" s="33"/>
-      <c r="P94" s="33"/>
-      <c r="Q94" s="33"/>
-      <c r="R94" s="33"/>
-      <c r="S94" s="33"/>
-      <c r="T94" s="33"/>
-      <c r="U94" s="33"/>
-      <c r="V94" s="34"/>
+      <c r="M94" s="39"/>
+      <c r="N94" s="39"/>
+      <c r="O94" s="39"/>
+      <c r="P94" s="39"/>
+      <c r="Q94" s="39"/>
+      <c r="R94" s="39"/>
+      <c r="S94" s="39"/>
+      <c r="T94" s="39"/>
+      <c r="U94" s="39"/>
+      <c r="V94" s="40"/>
     </row>
     <row r="95" spans="1:23">
       <c r="A95" s="24" t="s">
@@ -14708,6 +17298,29 @@
     </row>
   </sheetData>
   <mergeCells count="33">
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="D5:H5"/>
+    <mergeCell ref="I5:K5"/>
+    <mergeCell ref="A1:K2"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="I4:K4"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="D6:H7"/>
+    <mergeCell ref="I6:K6"/>
+    <mergeCell ref="A7:C8"/>
+    <mergeCell ref="I7:K7"/>
+    <mergeCell ref="D8:H8"/>
+    <mergeCell ref="I8:K8"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="D9:H9"/>
+    <mergeCell ref="I9:K9"/>
+    <mergeCell ref="A10:C11"/>
+    <mergeCell ref="D10:H10"/>
+    <mergeCell ref="I10:K10"/>
+    <mergeCell ref="D11:H11"/>
+    <mergeCell ref="I11:K11"/>
     <mergeCell ref="A57:K57"/>
     <mergeCell ref="L57:V57"/>
     <mergeCell ref="A94:K94"/>
@@ -14718,29 +17331,6 @@
     <mergeCell ref="L13:V13"/>
     <mergeCell ref="A50:K50"/>
     <mergeCell ref="L50:V50"/>
-    <mergeCell ref="A9:C9"/>
-    <mergeCell ref="D9:H9"/>
-    <mergeCell ref="I9:K9"/>
-    <mergeCell ref="A10:C11"/>
-    <mergeCell ref="D10:H10"/>
-    <mergeCell ref="I10:K10"/>
-    <mergeCell ref="D11:H11"/>
-    <mergeCell ref="I11:K11"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="D6:H7"/>
-    <mergeCell ref="I6:K6"/>
-    <mergeCell ref="A7:C8"/>
-    <mergeCell ref="I7:K7"/>
-    <mergeCell ref="D8:H8"/>
-    <mergeCell ref="I8:K8"/>
-    <mergeCell ref="A1:K2"/>
-    <mergeCell ref="A3:K3"/>
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="I4:K4"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="D5:H5"/>
-    <mergeCell ref="I5:K5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>